<commit_message>
CueSheet y Metadatos actualizados con Cyborg
</commit_message>
<xml_diff>
--- a/Docs/TDS/TablaMetadatos.xlsx
+++ b/Docs/TDS/TablaMetadatos.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Wasted-Racing\Docs\TDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\Wasted-Racing-master\Wasted-Racing-master\Docs\TDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="735" yWindow="840" windowWidth="26265" windowHeight="7980" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="7620" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="9" r:id="rId1"/>
@@ -20,17 +20,12 @@
     <sheet name="Metadatos D" sheetId="7" r:id="rId6"/>
     <sheet name="Metadatos V" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="402">
   <si>
     <t>ID</t>
   </si>
@@ -981,13 +976,268 @@
   </si>
   <si>
     <t>3.9</t>
+  </si>
+  <si>
+    <t>V-410</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P1ES_0.wav</t>
+  </si>
+  <si>
+    <t>Reducción de ruido, cambio de tono y eco</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>V-411</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P1ES_1.wav</t>
+  </si>
+  <si>
+    <t>V-415</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P1EN_0.wav</t>
+  </si>
+  <si>
+    <t>V-420</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P2ES_0.wav</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-425 </t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P2EN_0.wav</t>
+  </si>
+  <si>
+    <t>V-426</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P2EN_1.wav</t>
+  </si>
+  <si>
+    <t>V-430</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P3ES_0.wav</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>V-431</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P3ES_1.wav</t>
+  </si>
+  <si>
+    <t>V-435</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P3EN_0.wav</t>
+  </si>
+  <si>
+    <t>V-436</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P3EN_1.wav</t>
+  </si>
+  <si>
+    <t>V-440</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P4ES_0.wav</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>V-441</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P4ES_1.wav</t>
+  </si>
+  <si>
+    <t>V-445</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P4EN_0.wav</t>
+  </si>
+  <si>
+    <t>V-450</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P5ES_0.wav</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>V-451</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P5ES_1.wav</t>
+  </si>
+  <si>
+    <t>V-455</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P5EN_0.wav</t>
+  </si>
+  <si>
+    <t>V-456</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P5EN_1.wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-460 </t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P6ES_0.wav</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>V-461</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P6ES_1.wav</t>
+  </si>
+  <si>
+    <t>V-465</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P6EN_0.wav</t>
+  </si>
+  <si>
+    <t>V-466</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P6EN_1.wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-470 </t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P7ES_0.wav</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>V-475</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P7EN_0.wav</t>
+  </si>
+  <si>
+    <t>V-480</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P8ES_0.wav</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-485 </t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P8EN_0.wav</t>
+  </si>
+  <si>
+    <t>V-490</t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P9ES_0.wav</t>
+  </si>
+  <si>
+    <t>4.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-495 </t>
+  </si>
+  <si>
+    <t>Game/media/audio/voices/C-P9EN_0.wav</t>
+  </si>
+  <si>
+    <t>00.02.403</t>
+  </si>
+  <si>
+    <t>00.03.073</t>
+  </si>
+  <si>
+    <t>00.02.450</t>
+  </si>
+  <si>
+    <t>00.01.826</t>
+  </si>
+  <si>
+    <t>00.01.962</t>
+  </si>
+  <si>
+    <t>00.00.940</t>
+  </si>
+  <si>
+    <t>00.01.486</t>
+  </si>
+  <si>
+    <t>00.00.789</t>
+  </si>
+  <si>
+    <t>00.01.614</t>
+  </si>
+  <si>
+    <t>00.00.813</t>
+  </si>
+  <si>
+    <t>00.01.057</t>
+  </si>
+  <si>
+    <t>00.01.823</t>
+  </si>
+  <si>
+    <t>00.01.018</t>
+  </si>
+  <si>
+    <t>00.00.917</t>
+  </si>
+  <si>
+    <t>00.01.303</t>
+  </si>
+  <si>
+    <t>00.01.022</t>
+  </si>
+  <si>
+    <t>00.00.534</t>
+  </si>
+  <si>
+    <t>00.00.627</t>
+  </si>
+  <si>
+    <t>00.03.320</t>
+  </si>
+  <si>
+    <t>00.02.752</t>
+  </si>
+  <si>
+    <t>00.02.577</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1108,6 +1358,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8.8000000000000007"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1129,7 +1407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1432,8 +1710,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="70">
+  <cellStyleXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -1507,8 +1796,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1673,30 +1964,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1708,9 +1977,57 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="70"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="70" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="71" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="70" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="70" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="70" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="70" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="18" fillId="0" borderId="0" xfId="70" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="70" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="70" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="70" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="71" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="70" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="71" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="70" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" xfId="70" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="21" fontId="18" fillId="0" borderId="0" xfId="70" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="70" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="21" fontId="18" fillId="0" borderId="0" xfId="70" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="70">
+  <cellStyles count="72">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo 2" xfId="71"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
@@ -1780,6 +2097,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="70"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2083,7 +2401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -2253,12 +2571,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" location="'Metadatos M'!A1" display="Metadatos Música" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B7" location="'Metadatos A'!A1" display="Metadatos Ambientes" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B8" location="'Metadatos H'!A1" display="Metadatos HardFX" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B9" location="'Metadatos F'!A1" display="Metadatos Foleys" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B10" location="'Metadatos D'!A1" display="Metadatos Diseño" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B11" location="'Metadatos V'!A1" display="Metadatos Voces" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B6" location="'Metadatos M'!A1" display="Metadatos Música"/>
+    <hyperlink ref="B7" location="'Metadatos A'!A1" display="Metadatos Ambientes"/>
+    <hyperlink ref="B8" location="'Metadatos H'!A1" display="Metadatos HardFX"/>
+    <hyperlink ref="B9" location="'Metadatos F'!A1" display="Metadatos Foleys"/>
+    <hyperlink ref="B10" location="'Metadatos D'!A1" display="Metadatos Diseño"/>
+    <hyperlink ref="B11" location="'Metadatos V'!A1" display="Metadatos Voces"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2271,7 +2589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -2477,7 +2795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -2683,7 +3001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P17"/>
   <sheetViews>
     <sheetView topLeftCell="I1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -2961,12 +3279,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" xr:uid="{7446D709-72BD-4AED-822C-47971524E67A}"/>
-    <hyperlink ref="G5" r:id="rId2" xr:uid="{099D432C-2946-4073-925B-53FEA2A67976}"/>
-    <hyperlink ref="G6" r:id="rId3" xr:uid="{B4160306-D119-4FAF-8C23-D70122BE1BE1}"/>
-    <hyperlink ref="O4" r:id="rId4" location="'Menu principal'!B6" xr:uid="{BDE91E05-024E-4A3E-957B-74F6524BA8D6}"/>
-    <hyperlink ref="O5" r:id="rId5" location="'Menu principal'!B7" xr:uid="{CE5C9F75-58A8-4DE4-ACA0-F2732AA35A7C}"/>
-    <hyperlink ref="O6" r:id="rId6" location="'Menu principal'!B9" xr:uid="{B4E69740-3721-41B0-A6FF-5C8A82B9257F}"/>
+    <hyperlink ref="G4" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+    <hyperlink ref="G6" r:id="rId3"/>
+    <hyperlink ref="O4" r:id="rId4" location="'Menu principal'!B6"/>
+    <hyperlink ref="O5" r:id="rId5" location="'Menu principal'!B7"/>
+    <hyperlink ref="O6" r:id="rId6" location="'Menu principal'!B9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId7"/>
@@ -2979,7 +3297,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -3185,7 +3503,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -3391,11 +3709,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:O116"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="E106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I126" sqref="I126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3403,7 +3721,8 @@
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="54.85546875" customWidth="1"/>
-    <col min="4" max="6" width="3" style="19" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" style="19" customWidth="1"/>
+    <col min="5" max="6" width="3" style="19" customWidth="1"/>
     <col min="7" max="7" width="24.140625" customWidth="1"/>
     <col min="8" max="8" width="62.5703125" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" customWidth="1"/>
@@ -3503,7 +3822,7 @@
       </c>
       <c r="E4" s="26"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="90" t="s">
+      <c r="G4" s="82" t="s">
         <v>58</v>
       </c>
       <c r="H4" s="63" t="s">
@@ -3535,7 +3854,7 @@
       <c r="B5" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="85" t="s">
         <v>99</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3564,7 +3883,7 @@
       <c r="M5" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="N5" s="97">
+      <c r="N5" s="87">
         <v>-30</v>
       </c>
       <c r="O5" s="81" t="s">
@@ -3575,7 +3894,7 @@
       <c r="B6" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="85" t="s">
         <v>100</v>
       </c>
       <c r="D6" s="20" t="s">
@@ -3615,7 +3934,7 @@
       <c r="B7" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="95" t="s">
+      <c r="C7" s="85" t="s">
         <v>101</v>
       </c>
       <c r="D7" s="20" t="s">
@@ -3641,7 +3960,7 @@
       <c r="L7" s="48">
         <v>1</v>
       </c>
-      <c r="M7" s="96" t="s">
+      <c r="M7" s="86" t="s">
         <v>133</v>
       </c>
       <c r="N7" s="20">
@@ -3652,11 +3971,11 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="94"/>
-      <c r="B8" s="92" t="s">
+      <c r="A8" s="84"/>
+      <c r="B8" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="95" t="s">
+      <c r="C8" s="85" t="s">
         <v>102</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -3682,7 +4001,7 @@
       <c r="L8" s="48">
         <v>1</v>
       </c>
-      <c r="M8" s="96" t="s">
+      <c r="M8" s="86" t="s">
         <v>134</v>
       </c>
       <c r="N8" s="20">
@@ -3693,11 +4012,11 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="94"/>
-      <c r="B9" s="92" t="s">
+      <c r="A9" s="84"/>
+      <c r="B9" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="85" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="20" t="s">
@@ -3723,7 +4042,7 @@
       <c r="L9" s="48">
         <v>1</v>
       </c>
-      <c r="M9" s="96" t="s">
+      <c r="M9" s="86" t="s">
         <v>135</v>
       </c>
       <c r="N9" s="20">
@@ -3734,11 +4053,11 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="94"/>
-      <c r="B10" s="92" t="s">
+      <c r="A10" s="84"/>
+      <c r="B10" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="C10" s="85" t="s">
         <v>104</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -3764,7 +4083,7 @@
       <c r="L10" s="48">
         <v>1</v>
       </c>
-      <c r="M10" s="96" t="s">
+      <c r="M10" s="86" t="s">
         <v>136</v>
       </c>
       <c r="N10" s="20">
@@ -3775,11 +4094,11 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="94"/>
-      <c r="B11" s="92" t="s">
+      <c r="A11" s="84"/>
+      <c r="B11" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="85" t="s">
         <v>105</v>
       </c>
       <c r="D11" s="20" t="s">
@@ -3805,22 +4124,22 @@
       <c r="L11" s="48">
         <v>1</v>
       </c>
-      <c r="M11" s="96" t="s">
+      <c r="M11" s="86" t="s">
         <v>137</v>
       </c>
       <c r="N11" s="20">
         <v>-23</v>
       </c>
-      <c r="O11" s="98" t="s">
+      <c r="O11" s="88" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="94"/>
-      <c r="B12" s="92" t="s">
+      <c r="A12" s="84"/>
+      <c r="B12" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="85" t="s">
         <v>106</v>
       </c>
       <c r="D12" s="20" t="s">
@@ -3846,22 +4165,22 @@
       <c r="L12" s="48">
         <v>1</v>
       </c>
-      <c r="M12" s="96" t="s">
+      <c r="M12" s="86" t="s">
         <v>138</v>
       </c>
       <c r="N12" s="20">
         <v>-28</v>
       </c>
-      <c r="O12" s="98" t="s">
+      <c r="O12" s="88" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="94"/>
-      <c r="B13" s="92" t="s">
+      <c r="A13" s="84"/>
+      <c r="B13" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="85" t="s">
         <v>107</v>
       </c>
       <c r="D13" s="20" t="s">
@@ -3887,22 +4206,22 @@
       <c r="L13" s="48">
         <v>1</v>
       </c>
-      <c r="M13" s="96" t="s">
+      <c r="M13" s="86" t="s">
         <v>139</v>
       </c>
       <c r="N13" s="20">
         <v>-25</v>
       </c>
-      <c r="O13" s="98" t="s">
+      <c r="O13" s="88" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="94"/>
-      <c r="B14" s="92" t="s">
+      <c r="A14" s="84"/>
+      <c r="B14" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="85" t="s">
         <v>108</v>
       </c>
       <c r="D14" s="20" t="s">
@@ -3928,22 +4247,22 @@
       <c r="L14" s="48">
         <v>1</v>
       </c>
-      <c r="M14" s="96" t="s">
+      <c r="M14" s="86" t="s">
         <v>138</v>
       </c>
       <c r="N14" s="20">
         <v>-28</v>
       </c>
-      <c r="O14" s="98" t="s">
+      <c r="O14" s="88" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="94"/>
-      <c r="B15" s="92" t="s">
+      <c r="A15" s="84"/>
+      <c r="B15" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="85" t="s">
         <v>109</v>
       </c>
       <c r="D15" s="20" t="s">
@@ -3969,22 +4288,22 @@
       <c r="L15" s="48">
         <v>1</v>
       </c>
-      <c r="M15" s="96" t="s">
+      <c r="M15" s="86" t="s">
         <v>140</v>
       </c>
       <c r="N15" s="20">
         <v>-26</v>
       </c>
-      <c r="O15" s="98" t="s">
+      <c r="O15" s="88" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="94"/>
-      <c r="B16" s="92" t="s">
+      <c r="A16" s="84"/>
+      <c r="B16" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="95" t="s">
+      <c r="C16" s="85" t="s">
         <v>110</v>
       </c>
       <c r="D16" s="20" t="s">
@@ -4010,22 +4329,22 @@
       <c r="L16" s="48">
         <v>1</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="86" t="s">
         <v>141</v>
       </c>
       <c r="N16" s="20">
         <v>-25</v>
       </c>
-      <c r="O16" s="98" t="s">
+      <c r="O16" s="88" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="94"/>
-      <c r="B17" s="92" t="s">
+      <c r="A17" s="84"/>
+      <c r="B17" s="83" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="85" t="s">
         <v>111</v>
       </c>
       <c r="D17" s="20" t="s">
@@ -4051,22 +4370,22 @@
       <c r="L17" s="48">
         <v>1</v>
       </c>
-      <c r="M17" s="96" t="s">
+      <c r="M17" s="86" t="s">
         <v>133</v>
       </c>
       <c r="N17" s="20">
         <v>-25</v>
       </c>
-      <c r="O17" s="98" t="s">
+      <c r="O17" s="88" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="94"/>
-      <c r="B18" s="92" t="s">
+      <c r="A18" s="84"/>
+      <c r="B18" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="95" t="s">
+      <c r="C18" s="85" t="s">
         <v>112</v>
       </c>
       <c r="D18" s="20" t="s">
@@ -4092,22 +4411,22 @@
       <c r="L18" s="48">
         <v>1</v>
       </c>
-      <c r="M18" s="96" t="s">
+      <c r="M18" s="86" t="s">
         <v>142</v>
       </c>
       <c r="N18" s="20">
         <v>-24</v>
       </c>
-      <c r="O18" s="98" t="s">
+      <c r="O18" s="88" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="94"/>
-      <c r="B19" s="92" t="s">
+      <c r="A19" s="84"/>
+      <c r="B19" s="83" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="85" t="s">
         <v>113</v>
       </c>
       <c r="D19" s="20" t="s">
@@ -4133,22 +4452,22 @@
       <c r="L19" s="48">
         <v>1</v>
       </c>
-      <c r="M19" s="96" t="s">
+      <c r="M19" s="86" t="s">
         <v>143</v>
       </c>
       <c r="N19" s="20">
         <v>-26</v>
       </c>
-      <c r="O19" s="98" t="s">
+      <c r="O19" s="88" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="94"/>
-      <c r="B20" s="92" t="s">
+      <c r="A20" s="84"/>
+      <c r="B20" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="95" t="s">
+      <c r="C20" s="85" t="s">
         <v>114</v>
       </c>
       <c r="D20" s="20" t="s">
@@ -4174,22 +4493,22 @@
       <c r="L20" s="48">
         <v>1</v>
       </c>
-      <c r="M20" s="96" t="s">
+      <c r="M20" s="86" t="s">
         <v>134</v>
       </c>
       <c r="N20" s="20">
         <v>-29</v>
       </c>
-      <c r="O20" s="98" t="s">
+      <c r="O20" s="88" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="94"/>
-      <c r="B21" s="92" t="s">
+      <c r="A21" s="84"/>
+      <c r="B21" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="95" t="s">
+      <c r="C21" s="85" t="s">
         <v>115</v>
       </c>
       <c r="D21" s="20" t="s">
@@ -4215,22 +4534,22 @@
       <c r="L21" s="48">
         <v>1</v>
       </c>
-      <c r="M21" s="96" t="s">
+      <c r="M21" s="86" t="s">
         <v>144</v>
       </c>
       <c r="N21" s="20">
         <v>-24</v>
       </c>
-      <c r="O21" s="98" t="s">
+      <c r="O21" s="88" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="94"/>
-      <c r="B22" s="92" t="s">
+      <c r="A22" s="84"/>
+      <c r="B22" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="95" t="s">
+      <c r="C22" s="85" t="s">
         <v>116</v>
       </c>
       <c r="D22" s="20" t="s">
@@ -4256,22 +4575,22 @@
       <c r="L22" s="48">
         <v>1</v>
       </c>
-      <c r="M22" s="96" t="s">
+      <c r="M22" s="86" t="s">
         <v>142</v>
       </c>
       <c r="N22" s="20">
         <v>-27</v>
       </c>
-      <c r="O22" s="98" t="s">
+      <c r="O22" s="88" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="94"/>
-      <c r="B23" s="92" t="s">
+      <c r="A23" s="84"/>
+      <c r="B23" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="85" t="s">
         <v>117</v>
       </c>
       <c r="D23" s="20" t="s">
@@ -4297,22 +4616,22 @@
       <c r="L23" s="48">
         <v>1</v>
       </c>
-      <c r="M23" s="96" t="s">
+      <c r="M23" s="86" t="s">
         <v>145</v>
       </c>
       <c r="N23" s="20">
         <v>-26</v>
       </c>
-      <c r="O23" s="98" t="s">
+      <c r="O23" s="88" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="94"/>
-      <c r="B24" s="92" t="s">
+      <c r="A24" s="84"/>
+      <c r="B24" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="95" t="s">
+      <c r="C24" s="85" t="s">
         <v>118</v>
       </c>
       <c r="D24" s="20" t="s">
@@ -4338,22 +4657,22 @@
       <c r="L24" s="48">
         <v>1</v>
       </c>
-      <c r="M24" s="96" t="s">
+      <c r="M24" s="86" t="s">
         <v>146</v>
       </c>
       <c r="N24" s="20">
         <v>-26</v>
       </c>
-      <c r="O24" s="98" t="s">
+      <c r="O24" s="88" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="94"/>
-      <c r="B25" s="92" t="s">
+      <c r="A25" s="84"/>
+      <c r="B25" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="95" t="s">
+      <c r="C25" s="85" t="s">
         <v>119</v>
       </c>
       <c r="D25" s="20" t="s">
@@ -4379,22 +4698,22 @@
       <c r="L25" s="48">
         <v>1</v>
       </c>
-      <c r="M25" s="96" t="s">
+      <c r="M25" s="86" t="s">
         <v>147</v>
       </c>
       <c r="N25" s="20">
         <v>-23</v>
       </c>
-      <c r="O25" s="98" t="s">
+      <c r="O25" s="88" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="94"/>
-      <c r="B26" s="92" t="s">
+      <c r="A26" s="84"/>
+      <c r="B26" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="95" t="s">
+      <c r="C26" s="85" t="s">
         <v>120</v>
       </c>
       <c r="D26" s="20" t="s">
@@ -4420,22 +4739,22 @@
       <c r="L26" s="48">
         <v>1</v>
       </c>
-      <c r="M26" s="96" t="s">
+      <c r="M26" s="86" t="s">
         <v>148</v>
       </c>
       <c r="N26" s="20">
         <v>-27</v>
       </c>
-      <c r="O26" s="98" t="s">
+      <c r="O26" s="88" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="94"/>
-      <c r="B27" s="92" t="s">
+      <c r="A27" s="84"/>
+      <c r="B27" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="95" t="s">
+      <c r="C27" s="85" t="s">
         <v>121</v>
       </c>
       <c r="D27" s="20" t="s">
@@ -4461,22 +4780,22 @@
       <c r="L27" s="48">
         <v>1</v>
       </c>
-      <c r="M27" s="96" t="s">
+      <c r="M27" s="86" t="s">
         <v>149</v>
       </c>
       <c r="N27" s="20">
         <v>-29</v>
       </c>
-      <c r="O27" s="98" t="s">
+      <c r="O27" s="88" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="94"/>
-      <c r="B28" s="92" t="s">
+      <c r="A28" s="84"/>
+      <c r="B28" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="95" t="s">
+      <c r="C28" s="85" t="s">
         <v>122</v>
       </c>
       <c r="D28" s="20" t="s">
@@ -4502,22 +4821,22 @@
       <c r="L28" s="48">
         <v>1</v>
       </c>
-      <c r="M28" s="96" t="s">
+      <c r="M28" s="86" t="s">
         <v>150</v>
       </c>
       <c r="N28" s="20">
         <v>-29</v>
       </c>
-      <c r="O28" s="98" t="s">
+      <c r="O28" s="88" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="94"/>
-      <c r="B29" s="92" t="s">
+      <c r="A29" s="84"/>
+      <c r="B29" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="95" t="s">
+      <c r="C29" s="85" t="s">
         <v>123</v>
       </c>
       <c r="D29" s="20" t="s">
@@ -4543,22 +4862,22 @@
       <c r="L29" s="48">
         <v>1</v>
       </c>
-      <c r="M29" s="96" t="s">
+      <c r="M29" s="86" t="s">
         <v>151</v>
       </c>
       <c r="N29" s="20">
         <v>-28</v>
       </c>
-      <c r="O29" s="98" t="s">
+      <c r="O29" s="88" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="94"/>
-      <c r="B30" s="92" t="s">
+      <c r="A30" s="84"/>
+      <c r="B30" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="95" t="s">
+      <c r="C30" s="85" t="s">
         <v>124</v>
       </c>
       <c r="D30" s="20" t="s">
@@ -4584,22 +4903,22 @@
       <c r="L30" s="48">
         <v>1</v>
       </c>
-      <c r="M30" s="96" t="s">
+      <c r="M30" s="86" t="s">
         <v>152</v>
       </c>
       <c r="N30" s="20">
         <v>-22</v>
       </c>
-      <c r="O30" s="98" t="s">
+      <c r="O30" s="88" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="94"/>
-      <c r="B31" s="92" t="s">
+      <c r="A31" s="84"/>
+      <c r="B31" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="95" t="s">
+      <c r="C31" s="85" t="s">
         <v>126</v>
       </c>
       <c r="D31" s="20" t="s">
@@ -4625,22 +4944,22 @@
       <c r="L31" s="48">
         <v>1</v>
       </c>
-      <c r="M31" s="96" t="s">
+      <c r="M31" s="86" t="s">
         <v>154</v>
       </c>
       <c r="N31" s="20">
         <v>-20</v>
       </c>
-      <c r="O31" s="98" t="s">
+      <c r="O31" s="88" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="94"/>
-      <c r="B32" s="92" t="s">
+      <c r="A32" s="84"/>
+      <c r="B32" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="95" t="s">
+      <c r="C32" s="85" t="s">
         <v>127</v>
       </c>
       <c r="D32" s="20" t="s">
@@ -4666,22 +4985,22 @@
       <c r="L32" s="48">
         <v>1</v>
       </c>
-      <c r="M32" s="96" t="s">
+      <c r="M32" s="86" t="s">
         <v>153</v>
       </c>
       <c r="N32" s="20">
         <v>-19</v>
       </c>
-      <c r="O32" s="98" t="s">
+      <c r="O32" s="88" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="94"/>
-      <c r="B33" s="92" t="s">
+      <c r="A33" s="84"/>
+      <c r="B33" s="83" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="95" t="s">
+      <c r="C33" s="85" t="s">
         <v>125</v>
       </c>
       <c r="D33" s="20" t="s">
@@ -4707,22 +5026,22 @@
       <c r="L33" s="48">
         <v>1</v>
       </c>
-      <c r="M33" s="96" t="s">
+      <c r="M33" s="86" t="s">
         <v>152</v>
       </c>
       <c r="N33" s="20">
         <v>-22</v>
       </c>
-      <c r="O33" s="98" t="s">
+      <c r="O33" s="88" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="94"/>
-      <c r="B34" s="92" t="s">
+      <c r="A34" s="84"/>
+      <c r="B34" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="95" t="s">
+      <c r="C34" s="85" t="s">
         <v>128</v>
       </c>
       <c r="D34" s="20" t="s">
@@ -4748,22 +5067,22 @@
       <c r="L34" s="48">
         <v>1</v>
       </c>
-      <c r="M34" s="96" t="s">
+      <c r="M34" s="86" t="s">
         <v>154</v>
       </c>
       <c r="N34" s="20">
         <v>-20</v>
       </c>
-      <c r="O34" s="98" t="s">
+      <c r="O34" s="88" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="94"/>
-      <c r="B35" s="92" t="s">
+      <c r="A35" s="84"/>
+      <c r="B35" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="95" t="s">
+      <c r="C35" s="85" t="s">
         <v>129</v>
       </c>
       <c r="D35" s="20" t="s">
@@ -4789,22 +5108,22 @@
       <c r="L35" s="48">
         <v>1</v>
       </c>
-      <c r="M35" s="96" t="s">
+      <c r="M35" s="86" t="s">
         <v>153</v>
       </c>
       <c r="N35" s="20">
         <v>-19</v>
       </c>
-      <c r="O35" s="98" t="s">
+      <c r="O35" s="88" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="94"/>
-      <c r="B36" s="92" t="s">
+      <c r="A36" s="84"/>
+      <c r="B36" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="C36" s="95" t="s">
+      <c r="C36" s="85" t="s">
         <v>155</v>
       </c>
       <c r="D36" s="20" t="s">
@@ -4830,22 +5149,22 @@
       <c r="L36" s="48">
         <v>1</v>
       </c>
-      <c r="M36" s="96" t="s">
+      <c r="M36" s="86" t="s">
         <v>131</v>
       </c>
       <c r="N36" s="20">
         <v>-15</v>
       </c>
-      <c r="O36" s="98" t="s">
+      <c r="O36" s="88" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="94"/>
-      <c r="B37" s="92" t="s">
+      <c r="A37" s="84"/>
+      <c r="B37" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="C37" s="95" t="s">
+      <c r="C37" s="85" t="s">
         <v>156</v>
       </c>
       <c r="D37" s="20" t="s">
@@ -4871,22 +5190,22 @@
       <c r="L37" s="48">
         <v>1</v>
       </c>
-      <c r="M37" s="96" t="s">
+      <c r="M37" s="86" t="s">
         <v>209</v>
       </c>
       <c r="N37" s="20">
         <v>-15</v>
       </c>
-      <c r="O37" s="98" t="s">
+      <c r="O37" s="88" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="94"/>
-      <c r="B38" s="92" t="s">
+      <c r="A38" s="84"/>
+      <c r="B38" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="C38" s="95" t="s">
+      <c r="C38" s="85" t="s">
         <v>157</v>
       </c>
       <c r="D38" s="20" t="s">
@@ -4912,22 +5231,22 @@
       <c r="L38" s="48">
         <v>1</v>
       </c>
-      <c r="M38" s="96" t="s">
+      <c r="M38" s="86" t="s">
         <v>210</v>
       </c>
       <c r="N38" s="20">
         <v>-19</v>
       </c>
-      <c r="O38" s="98" t="s">
+      <c r="O38" s="88" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="94"/>
-      <c r="B39" s="92" t="s">
+      <c r="A39" s="84"/>
+      <c r="B39" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="C39" s="95" t="s">
+      <c r="C39" s="85" t="s">
         <v>158</v>
       </c>
       <c r="D39" s="20" t="s">
@@ -4953,22 +5272,22 @@
       <c r="L39" s="48">
         <v>1</v>
       </c>
-      <c r="M39" s="96" t="s">
+      <c r="M39" s="86" t="s">
         <v>211</v>
       </c>
       <c r="N39" s="20">
         <v>-17</v>
       </c>
-      <c r="O39" s="98" t="s">
+      <c r="O39" s="88" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="94"/>
-      <c r="B40" s="92" t="s">
+      <c r="A40" s="84"/>
+      <c r="B40" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="C40" s="95" t="s">
+      <c r="C40" s="85" t="s">
         <v>159</v>
       </c>
       <c r="D40" s="20" t="s">
@@ -4994,22 +5313,22 @@
       <c r="L40" s="48">
         <v>1</v>
       </c>
-      <c r="M40" s="96" t="s">
+      <c r="M40" s="86" t="s">
         <v>137</v>
       </c>
       <c r="N40" s="20">
         <v>-20</v>
       </c>
-      <c r="O40" s="98" t="s">
+      <c r="O40" s="88" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="94"/>
-      <c r="B41" s="92" t="s">
+      <c r="A41" s="84"/>
+      <c r="B41" s="83" t="s">
         <v>187</v>
       </c>
-      <c r="C41" s="95" t="s">
+      <c r="C41" s="85" t="s">
         <v>160</v>
       </c>
       <c r="D41" s="20" t="s">
@@ -5035,22 +5354,22 @@
       <c r="L41" s="48">
         <v>1</v>
       </c>
-      <c r="M41" s="96" t="s">
+      <c r="M41" s="86" t="s">
         <v>130</v>
       </c>
       <c r="N41" s="20">
         <v>-18</v>
       </c>
-      <c r="O41" s="98" t="s">
+      <c r="O41" s="88" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="94"/>
-      <c r="B42" s="92" t="s">
+      <c r="A42" s="84"/>
+      <c r="B42" s="83" t="s">
         <v>188</v>
       </c>
-      <c r="C42" s="95" t="s">
+      <c r="C42" s="85" t="s">
         <v>161</v>
       </c>
       <c r="D42" s="20" t="s">
@@ -5076,22 +5395,22 @@
       <c r="L42" s="48">
         <v>1</v>
       </c>
-      <c r="M42" s="96" t="s">
+      <c r="M42" s="86" t="s">
         <v>212</v>
       </c>
       <c r="N42" s="20">
         <v>-25</v>
       </c>
-      <c r="O42" s="98" t="s">
+      <c r="O42" s="88" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="94"/>
-      <c r="B43" s="92" t="s">
+      <c r="A43" s="84"/>
+      <c r="B43" s="83" t="s">
         <v>189</v>
       </c>
-      <c r="C43" s="95" t="s">
+      <c r="C43" s="85" t="s">
         <v>162</v>
       </c>
       <c r="D43" s="20" t="s">
@@ -5117,22 +5436,22 @@
       <c r="L43" s="48">
         <v>1</v>
       </c>
-      <c r="M43" s="96" t="s">
+      <c r="M43" s="86" t="s">
         <v>213</v>
       </c>
       <c r="N43" s="20">
         <v>-14</v>
       </c>
-      <c r="O43" s="98" t="s">
+      <c r="O43" s="88" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="94"/>
-      <c r="B44" s="92" t="s">
+      <c r="A44" s="84"/>
+      <c r="B44" s="83" t="s">
         <v>190</v>
       </c>
-      <c r="C44" s="95" t="s">
+      <c r="C44" s="85" t="s">
         <v>164</v>
       </c>
       <c r="D44" s="20" t="s">
@@ -5158,22 +5477,22 @@
       <c r="L44" s="48">
         <v>1</v>
       </c>
-      <c r="M44" s="96" t="s">
+      <c r="M44" s="86" t="s">
         <v>214</v>
       </c>
       <c r="N44" s="20">
         <v>-13</v>
       </c>
-      <c r="O44" s="98" t="s">
+      <c r="O44" s="88" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="94"/>
-      <c r="B45" s="92" t="s">
+      <c r="A45" s="84"/>
+      <c r="B45" s="83" t="s">
         <v>191</v>
       </c>
-      <c r="C45" s="95" t="s">
+      <c r="C45" s="85" t="s">
         <v>165</v>
       </c>
       <c r="D45" s="20" t="s">
@@ -5199,22 +5518,22 @@
       <c r="L45" s="48">
         <v>1</v>
       </c>
-      <c r="M45" s="96" t="s">
+      <c r="M45" s="86" t="s">
         <v>135</v>
       </c>
       <c r="N45" s="20">
         <v>-20</v>
       </c>
-      <c r="O45" s="98" t="s">
+      <c r="O45" s="88" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="94"/>
-      <c r="B46" s="92" t="s">
+      <c r="A46" s="84"/>
+      <c r="B46" s="83" t="s">
         <v>192</v>
       </c>
-      <c r="C46" s="95" t="s">
+      <c r="C46" s="85" t="s">
         <v>163</v>
       </c>
       <c r="D46" s="20" t="s">
@@ -5240,22 +5559,22 @@
       <c r="L46" s="48">
         <v>1</v>
       </c>
-      <c r="M46" s="96" t="s">
+      <c r="M46" s="86" t="s">
         <v>215</v>
       </c>
       <c r="N46" s="20">
         <v>-14</v>
       </c>
-      <c r="O46" s="98" t="s">
+      <c r="O46" s="88" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="94"/>
-      <c r="B47" s="92" t="s">
+      <c r="A47" s="84"/>
+      <c r="B47" s="83" t="s">
         <v>193</v>
       </c>
-      <c r="C47" s="95" t="s">
+      <c r="C47" s="85" t="s">
         <v>166</v>
       </c>
       <c r="D47" s="20" t="s">
@@ -5281,22 +5600,22 @@
       <c r="L47" s="48">
         <v>1</v>
       </c>
-      <c r="M47" s="96" t="s">
+      <c r="M47" s="86" t="s">
         <v>137</v>
       </c>
       <c r="N47" s="20">
         <v>-11</v>
       </c>
-      <c r="O47" s="98" t="s">
+      <c r="O47" s="88" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="94"/>
-      <c r="B48" s="92" t="s">
+      <c r="A48" s="84"/>
+      <c r="B48" s="83" t="s">
         <v>194</v>
       </c>
-      <c r="C48" s="95" t="s">
+      <c r="C48" s="85" t="s">
         <v>167</v>
       </c>
       <c r="D48" s="20" t="s">
@@ -5322,22 +5641,22 @@
       <c r="L48" s="48">
         <v>1</v>
       </c>
-      <c r="M48" s="96" t="s">
+      <c r="M48" s="86" t="s">
         <v>216</v>
       </c>
       <c r="N48" s="20">
         <v>-13</v>
       </c>
-      <c r="O48" s="98" t="s">
+      <c r="O48" s="88" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="94"/>
-      <c r="B49" s="92" t="s">
+      <c r="A49" s="84"/>
+      <c r="B49" s="83" t="s">
         <v>195</v>
       </c>
-      <c r="C49" s="95" t="s">
+      <c r="C49" s="85" t="s">
         <v>168</v>
       </c>
       <c r="D49" s="20" t="s">
@@ -5363,22 +5682,22 @@
       <c r="L49" s="48">
         <v>1</v>
       </c>
-      <c r="M49" s="96" t="s">
+      <c r="M49" s="86" t="s">
         <v>212</v>
       </c>
       <c r="N49" s="20">
         <v>-11</v>
       </c>
-      <c r="O49" s="98" t="s">
+      <c r="O49" s="88" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="94"/>
-      <c r="B50" s="92" t="s">
+      <c r="A50" s="84"/>
+      <c r="B50" s="83" t="s">
         <v>196</v>
       </c>
-      <c r="C50" s="95" t="s">
+      <c r="C50" s="85" t="s">
         <v>169</v>
       </c>
       <c r="D50" s="20" t="s">
@@ -5404,22 +5723,22 @@
       <c r="L50" s="48">
         <v>1</v>
       </c>
-      <c r="M50" s="96" t="s">
+      <c r="M50" s="86" t="s">
         <v>137</v>
       </c>
       <c r="N50" s="20">
         <v>-19</v>
       </c>
-      <c r="O50" s="98" t="s">
+      <c r="O50" s="88" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="94"/>
-      <c r="B51" s="92" t="s">
+      <c r="A51" s="84"/>
+      <c r="B51" s="83" t="s">
         <v>197</v>
       </c>
-      <c r="C51" s="95" t="s">
+      <c r="C51" s="85" t="s">
         <v>170</v>
       </c>
       <c r="D51" s="20" t="s">
@@ -5445,22 +5764,22 @@
       <c r="L51" s="48">
         <v>1</v>
       </c>
-      <c r="M51" s="96" t="s">
+      <c r="M51" s="86" t="s">
         <v>137</v>
       </c>
       <c r="N51" s="20">
         <v>-19</v>
       </c>
-      <c r="O51" s="98" t="s">
+      <c r="O51" s="88" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="94"/>
-      <c r="B52" s="92" t="s">
+      <c r="A52" s="84"/>
+      <c r="B52" s="83" t="s">
         <v>198</v>
       </c>
-      <c r="C52" s="95" t="s">
+      <c r="C52" s="85" t="s">
         <v>171</v>
       </c>
       <c r="D52" s="20" t="s">
@@ -5486,22 +5805,22 @@
       <c r="L52" s="48">
         <v>1</v>
       </c>
-      <c r="M52" s="96" t="s">
+      <c r="M52" s="86" t="s">
         <v>137</v>
       </c>
       <c r="N52" s="20">
         <v>-19</v>
       </c>
-      <c r="O52" s="98" t="s">
+      <c r="O52" s="88" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="94"/>
-      <c r="B53" s="92" t="s">
+      <c r="A53" s="84"/>
+      <c r="B53" s="83" t="s">
         <v>199</v>
       </c>
-      <c r="C53" s="95" t="s">
+      <c r="C53" s="85" t="s">
         <v>173</v>
       </c>
       <c r="D53" s="20" t="s">
@@ -5527,22 +5846,22 @@
       <c r="L53" s="48">
         <v>1</v>
       </c>
-      <c r="M53" s="96" t="s">
+      <c r="M53" s="86" t="s">
         <v>215</v>
       </c>
       <c r="N53" s="20">
         <v>-20</v>
       </c>
-      <c r="O53" s="98" t="s">
+      <c r="O53" s="88" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="94"/>
-      <c r="B54" s="92" t="s">
+      <c r="A54" s="84"/>
+      <c r="B54" s="83" t="s">
         <v>200</v>
       </c>
-      <c r="C54" s="95" t="s">
+      <c r="C54" s="85" t="s">
         <v>172</v>
       </c>
       <c r="D54" s="20" t="s">
@@ -5568,22 +5887,22 @@
       <c r="L54" s="48">
         <v>1</v>
       </c>
-      <c r="M54" s="96" t="s">
+      <c r="M54" s="86" t="s">
         <v>137</v>
       </c>
       <c r="N54" s="20">
         <v>-19</v>
       </c>
-      <c r="O54" s="98" t="s">
+      <c r="O54" s="88" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="94"/>
-      <c r="B55" s="92" t="s">
+      <c r="A55" s="84"/>
+      <c r="B55" s="83" t="s">
         <v>201</v>
       </c>
-      <c r="C55" s="95" t="s">
+      <c r="C55" s="85" t="s">
         <v>174</v>
       </c>
       <c r="D55" s="20" t="s">
@@ -5609,22 +5928,22 @@
       <c r="L55" s="48">
         <v>1</v>
       </c>
-      <c r="M55" s="96" t="s">
+      <c r="M55" s="86" t="s">
         <v>215</v>
       </c>
       <c r="N55" s="20">
         <v>-20</v>
       </c>
-      <c r="O55" s="98" t="s">
+      <c r="O55" s="88" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="94"/>
-      <c r="B56" s="92" t="s">
+      <c r="A56" s="84"/>
+      <c r="B56" s="83" t="s">
         <v>202</v>
       </c>
-      <c r="C56" s="95" t="s">
+      <c r="C56" s="85" t="s">
         <v>175</v>
       </c>
       <c r="D56" s="20" t="s">
@@ -5650,22 +5969,22 @@
       <c r="L56" s="48">
         <v>1</v>
       </c>
-      <c r="M56" s="96" t="s">
+      <c r="M56" s="86" t="s">
         <v>217</v>
       </c>
       <c r="N56" s="20">
         <v>-15</v>
       </c>
-      <c r="O56" s="98" t="s">
+      <c r="O56" s="88" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="94"/>
-      <c r="B57" s="92" t="s">
+      <c r="A57" s="84"/>
+      <c r="B57" s="83" t="s">
         <v>203</v>
       </c>
-      <c r="C57" s="95" t="s">
+      <c r="C57" s="85" t="s">
         <v>176</v>
       </c>
       <c r="D57" s="20" t="s">
@@ -5691,22 +6010,22 @@
       <c r="L57" s="48">
         <v>1</v>
       </c>
-      <c r="M57" s="96" t="s">
+      <c r="M57" s="86" t="s">
         <v>218</v>
       </c>
       <c r="N57" s="20">
         <v>-15</v>
       </c>
-      <c r="O57" s="98" t="s">
+      <c r="O57" s="88" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="94"/>
-      <c r="B58" s="92" t="s">
+      <c r="A58" s="84"/>
+      <c r="B58" s="83" t="s">
         <v>204</v>
       </c>
-      <c r="C58" s="95" t="s">
+      <c r="C58" s="85" t="s">
         <v>177</v>
       </c>
       <c r="D58" s="20" t="s">
@@ -5732,22 +6051,22 @@
       <c r="L58" s="48">
         <v>1</v>
       </c>
-      <c r="M58" s="96" t="s">
+      <c r="M58" s="86" t="s">
         <v>217</v>
       </c>
       <c r="N58" s="20">
         <v>-15</v>
       </c>
-      <c r="O58" s="98" t="s">
+      <c r="O58" s="88" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="94"/>
-      <c r="B59" s="92" t="s">
+      <c r="A59" s="84"/>
+      <c r="B59" s="83" t="s">
         <v>205</v>
       </c>
-      <c r="C59" s="95" t="s">
+      <c r="C59" s="85" t="s">
         <v>178</v>
       </c>
       <c r="D59" s="20" t="s">
@@ -5773,22 +6092,22 @@
       <c r="L59" s="48">
         <v>1</v>
       </c>
-      <c r="M59" s="96" t="s">
+      <c r="M59" s="86" t="s">
         <v>219</v>
       </c>
       <c r="N59" s="20">
         <v>-15</v>
       </c>
-      <c r="O59" s="98" t="s">
+      <c r="O59" s="88" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="94"/>
-      <c r="B60" s="92" t="s">
+      <c r="A60" s="84"/>
+      <c r="B60" s="83" t="s">
         <v>206</v>
       </c>
-      <c r="C60" s="95" t="s">
+      <c r="C60" s="85" t="s">
         <v>179</v>
       </c>
       <c r="D60" s="20" t="s">
@@ -5814,22 +6133,22 @@
       <c r="L60" s="48">
         <v>1</v>
       </c>
-      <c r="M60" s="96" t="s">
+      <c r="M60" s="86" t="s">
         <v>220</v>
       </c>
       <c r="N60" s="20">
         <v>-14</v>
       </c>
-      <c r="O60" s="98" t="s">
+      <c r="O60" s="88" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="94"/>
-      <c r="B61" s="92" t="s">
+      <c r="A61" s="84"/>
+      <c r="B61" s="83" t="s">
         <v>207</v>
       </c>
-      <c r="C61" s="95" t="s">
+      <c r="C61" s="85" t="s">
         <v>180</v>
       </c>
       <c r="D61" s="20" t="s">
@@ -5855,22 +6174,22 @@
       <c r="L61" s="48">
         <v>1</v>
       </c>
-      <c r="M61" s="96" t="s">
+      <c r="M61" s="86" t="s">
         <v>154</v>
       </c>
       <c r="N61" s="20">
         <v>-13</v>
       </c>
-      <c r="O61" s="98" t="s">
+      <c r="O61" s="88" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="94"/>
-      <c r="B62" s="92" t="s">
+      <c r="A62" s="84"/>
+      <c r="B62" s="83" t="s">
         <v>208</v>
       </c>
-      <c r="C62" s="95" t="s">
+      <c r="C62" s="85" t="s">
         <v>181</v>
       </c>
       <c r="D62" s="20" t="s">
@@ -5896,22 +6215,22 @@
       <c r="L62" s="48">
         <v>1</v>
       </c>
-      <c r="M62" s="96" t="s">
+      <c r="M62" s="86" t="s">
         <v>154</v>
       </c>
       <c r="N62" s="20">
         <v>-13</v>
       </c>
-      <c r="O62" s="98" t="s">
+      <c r="O62" s="88" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="94"/>
-      <c r="B63" s="92" t="s">
+      <c r="A63" s="84"/>
+      <c r="B63" s="83" t="s">
         <v>230</v>
       </c>
-      <c r="C63" s="95" t="s">
+      <c r="C63" s="85" t="s">
         <v>263</v>
       </c>
       <c r="D63" s="20" t="s">
@@ -5937,22 +6256,22 @@
       <c r="L63" s="48">
         <v>1</v>
       </c>
-      <c r="M63" s="96" t="s">
+      <c r="M63" s="86" t="s">
         <v>297</v>
       </c>
       <c r="N63" s="20">
         <v>-25</v>
       </c>
-      <c r="O63" s="98" t="s">
+      <c r="O63" s="88" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="94"/>
-      <c r="B64" s="92" t="s">
+      <c r="A64" s="84"/>
+      <c r="B64" s="83" t="s">
         <v>231</v>
       </c>
-      <c r="C64" s="95" t="s">
+      <c r="C64" s="85" t="s">
         <v>264</v>
       </c>
       <c r="D64" s="20" t="s">
@@ -5978,22 +6297,22 @@
       <c r="L64" s="48">
         <v>1</v>
       </c>
-      <c r="M64" s="96" t="s">
+      <c r="M64" s="86" t="s">
         <v>297</v>
       </c>
       <c r="N64" s="20">
         <v>-25</v>
       </c>
-      <c r="O64" s="98" t="s">
+      <c r="O64" s="88" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="94"/>
-      <c r="B65" s="92" t="s">
+      <c r="A65" s="84"/>
+      <c r="B65" s="83" t="s">
         <v>232</v>
       </c>
-      <c r="C65" s="95" t="s">
+      <c r="C65" s="85" t="s">
         <v>265</v>
       </c>
       <c r="D65" s="20" t="s">
@@ -6019,22 +6338,22 @@
       <c r="L65" s="48">
         <v>1</v>
       </c>
-      <c r="M65" s="96" t="s">
+      <c r="M65" s="86" t="s">
         <v>216</v>
       </c>
       <c r="N65" s="20">
         <v>-25</v>
       </c>
-      <c r="O65" s="98" t="s">
+      <c r="O65" s="88" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="94"/>
-      <c r="B66" s="92" t="s">
+      <c r="A66" s="84"/>
+      <c r="B66" s="83" t="s">
         <v>233</v>
       </c>
-      <c r="C66" s="95" t="s">
+      <c r="C66" s="85" t="s">
         <v>266</v>
       </c>
       <c r="D66" s="20" t="s">
@@ -6060,22 +6379,22 @@
       <c r="L66" s="48">
         <v>1</v>
       </c>
-      <c r="M66" s="96" t="s">
+      <c r="M66" s="86" t="s">
         <v>137</v>
       </c>
       <c r="N66" s="20">
         <v>-25</v>
       </c>
-      <c r="O66" s="98" t="s">
+      <c r="O66" s="88" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="94"/>
-      <c r="B67" s="92" t="s">
+      <c r="A67" s="84"/>
+      <c r="B67" s="83" t="s">
         <v>234</v>
       </c>
-      <c r="C67" s="95" t="s">
+      <c r="C67" s="85" t="s">
         <v>267</v>
       </c>
       <c r="D67" s="20" t="s">
@@ -6101,22 +6420,22 @@
       <c r="L67" s="48">
         <v>1</v>
       </c>
-      <c r="M67" s="96" t="s">
+      <c r="M67" s="86" t="s">
         <v>216</v>
       </c>
       <c r="N67" s="20">
         <v>-25</v>
       </c>
-      <c r="O67" s="98" t="s">
+      <c r="O67" s="88" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="94"/>
-      <c r="B68" s="92" t="s">
+      <c r="A68" s="84"/>
+      <c r="B68" s="83" t="s">
         <v>235</v>
       </c>
-      <c r="C68" s="95" t="s">
+      <c r="C68" s="85" t="s">
         <v>268</v>
       </c>
       <c r="D68" s="20" t="s">
@@ -6142,22 +6461,22 @@
       <c r="L68" s="48">
         <v>1</v>
       </c>
-      <c r="M68" s="96" t="s">
+      <c r="M68" s="86" t="s">
         <v>299</v>
       </c>
       <c r="N68" s="20">
         <v>-25</v>
       </c>
-      <c r="O68" s="98" t="s">
+      <c r="O68" s="88" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="94"/>
-      <c r="B69" s="92" t="s">
+      <c r="A69" s="84"/>
+      <c r="B69" s="83" t="s">
         <v>236</v>
       </c>
-      <c r="C69" s="95" t="s">
+      <c r="C69" s="85" t="s">
         <v>269</v>
       </c>
       <c r="D69" s="20" t="s">
@@ -6183,22 +6502,22 @@
       <c r="L69" s="48">
         <v>1</v>
       </c>
-      <c r="M69" s="96" t="s">
+      <c r="M69" s="86" t="s">
         <v>216</v>
       </c>
       <c r="N69" s="20">
         <v>-26</v>
       </c>
-      <c r="O69" s="98" t="s">
+      <c r="O69" s="88" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="94"/>
-      <c r="B70" s="92" t="s">
+      <c r="A70" s="84"/>
+      <c r="B70" s="83" t="s">
         <v>237</v>
       </c>
-      <c r="C70" s="95" t="s">
+      <c r="C70" s="85" t="s">
         <v>270</v>
       </c>
       <c r="D70" s="20" t="s">
@@ -6224,22 +6543,22 @@
       <c r="L70" s="48">
         <v>1</v>
       </c>
-      <c r="M70" s="96" t="s">
+      <c r="M70" s="86" t="s">
         <v>153</v>
       </c>
       <c r="N70" s="20">
         <v>-31</v>
       </c>
-      <c r="O70" s="98" t="s">
+      <c r="O70" s="88" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="94"/>
-      <c r="B71" s="92" t="s">
+      <c r="A71" s="84"/>
+      <c r="B71" s="83" t="s">
         <v>238</v>
       </c>
-      <c r="C71" s="95" t="s">
+      <c r="C71" s="85" t="s">
         <v>271</v>
       </c>
       <c r="D71" s="20" t="s">
@@ -6265,22 +6584,22 @@
       <c r="L71" s="48">
         <v>1</v>
       </c>
-      <c r="M71" s="96" t="s">
+      <c r="M71" s="86" t="s">
         <v>300</v>
       </c>
       <c r="N71" s="20">
         <v>-26</v>
       </c>
-      <c r="O71" s="98" t="s">
+      <c r="O71" s="88" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="94"/>
-      <c r="B72" s="92" t="s">
+      <c r="A72" s="84"/>
+      <c r="B72" s="83" t="s">
         <v>239</v>
       </c>
-      <c r="C72" s="95" t="s">
+      <c r="C72" s="85" t="s">
         <v>272</v>
       </c>
       <c r="D72" s="20" t="s">
@@ -6306,22 +6625,22 @@
       <c r="L72" s="48">
         <v>1</v>
       </c>
-      <c r="M72" s="96" t="s">
+      <c r="M72" s="86" t="s">
         <v>153</v>
       </c>
       <c r="N72" s="20">
         <v>-30</v>
       </c>
-      <c r="O72" s="98" t="s">
+      <c r="O72" s="88" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="94"/>
-      <c r="B73" s="92" t="s">
+      <c r="A73" s="84"/>
+      <c r="B73" s="83" t="s">
         <v>240</v>
       </c>
-      <c r="C73" s="95" t="s">
+      <c r="C73" s="85" t="s">
         <v>273</v>
       </c>
       <c r="D73" s="20" t="s">
@@ -6347,22 +6666,22 @@
       <c r="L73" s="48">
         <v>1</v>
       </c>
-      <c r="M73" s="96" t="s">
+      <c r="M73" s="86" t="s">
         <v>144</v>
       </c>
       <c r="N73" s="20">
         <v>-27</v>
       </c>
-      <c r="O73" s="98" t="s">
+      <c r="O73" s="88" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A74" s="94"/>
-      <c r="B74" s="92" t="s">
+      <c r="A74" s="84"/>
+      <c r="B74" s="83" t="s">
         <v>241</v>
       </c>
-      <c r="C74" s="95" t="s">
+      <c r="C74" s="85" t="s">
         <v>274</v>
       </c>
       <c r="D74" s="20" t="s">
@@ -6388,22 +6707,22 @@
       <c r="L74" s="48">
         <v>1</v>
       </c>
-      <c r="M74" s="96" t="s">
+      <c r="M74" s="86" t="s">
         <v>133</v>
       </c>
       <c r="N74" s="20">
         <v>-26</v>
       </c>
-      <c r="O74" s="98" t="s">
+      <c r="O74" s="88" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" s="94"/>
-      <c r="B75" s="92" t="s">
+      <c r="A75" s="84"/>
+      <c r="B75" s="83" t="s">
         <v>242</v>
       </c>
-      <c r="C75" s="95" t="s">
+      <c r="C75" s="85" t="s">
         <v>275</v>
       </c>
       <c r="D75" s="20" t="s">
@@ -6429,22 +6748,22 @@
       <c r="L75" s="48">
         <v>1</v>
       </c>
-      <c r="M75" s="96" t="s">
+      <c r="M75" s="86" t="s">
         <v>212</v>
       </c>
       <c r="N75" s="20">
         <v>-27</v>
       </c>
-      <c r="O75" s="98" t="s">
+      <c r="O75" s="88" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76" s="94"/>
-      <c r="B76" s="92" t="s">
+      <c r="A76" s="84"/>
+      <c r="B76" s="83" t="s">
         <v>243</v>
       </c>
-      <c r="C76" s="95" t="s">
+      <c r="C76" s="85" t="s">
         <v>276</v>
       </c>
       <c r="D76" s="20" t="s">
@@ -6470,22 +6789,22 @@
       <c r="L76" s="48">
         <v>1</v>
       </c>
-      <c r="M76" s="96" t="s">
+      <c r="M76" s="86" t="s">
         <v>133</v>
       </c>
       <c r="N76" s="20">
         <v>-34</v>
       </c>
-      <c r="O76" s="98" t="s">
+      <c r="O76" s="88" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A77" s="94"/>
-      <c r="B77" s="92" t="s">
+      <c r="A77" s="84"/>
+      <c r="B77" s="83" t="s">
         <v>244</v>
       </c>
-      <c r="C77" s="95" t="s">
+      <c r="C77" s="85" t="s">
         <v>278</v>
       </c>
       <c r="D77" s="20" t="s">
@@ -6511,22 +6830,22 @@
       <c r="L77" s="48">
         <v>1</v>
       </c>
-      <c r="M77" s="96" t="s">
+      <c r="M77" s="86" t="s">
         <v>215</v>
       </c>
       <c r="N77" s="20">
         <v>-20</v>
       </c>
-      <c r="O77" s="98" t="s">
+      <c r="O77" s="88" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A78" s="94"/>
-      <c r="B78" s="92" t="s">
+      <c r="A78" s="84"/>
+      <c r="B78" s="83" t="s">
         <v>245</v>
       </c>
-      <c r="C78" s="95" t="s">
+      <c r="C78" s="85" t="s">
         <v>279</v>
       </c>
       <c r="D78" s="20" t="s">
@@ -6552,22 +6871,22 @@
       <c r="L78" s="48">
         <v>1</v>
       </c>
-      <c r="M78" s="96" t="s">
+      <c r="M78" s="86" t="s">
         <v>212</v>
       </c>
       <c r="N78" s="20">
         <v>-29</v>
       </c>
-      <c r="O78" s="98" t="s">
+      <c r="O78" s="88" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A79" s="94"/>
-      <c r="B79" s="92" t="s">
+      <c r="A79" s="84"/>
+      <c r="B79" s="83" t="s">
         <v>246</v>
       </c>
-      <c r="C79" s="95" t="s">
+      <c r="C79" s="85" t="s">
         <v>277</v>
       </c>
       <c r="D79" s="20" t="s">
@@ -6599,16 +6918,16 @@
       <c r="N79" s="20">
         <v>-28</v>
       </c>
-      <c r="O79" s="98" t="s">
+      <c r="O79" s="88" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A80" s="94"/>
-      <c r="B80" s="92" t="s">
+      <c r="A80" s="84"/>
+      <c r="B80" s="83" t="s">
         <v>247</v>
       </c>
-      <c r="C80" s="95" t="s">
+      <c r="C80" s="85" t="s">
         <v>280</v>
       </c>
       <c r="D80" s="20" t="s">
@@ -6634,22 +6953,22 @@
       <c r="L80" s="48">
         <v>1</v>
       </c>
-      <c r="M80" s="96" t="s">
+      <c r="M80" s="86" t="s">
         <v>137</v>
       </c>
       <c r="N80" s="20">
         <v>-19</v>
       </c>
-      <c r="O80" s="98" t="s">
+      <c r="O80" s="88" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A81" s="94"/>
-      <c r="B81" s="92" t="s">
+      <c r="A81" s="84"/>
+      <c r="B81" s="83" t="s">
         <v>248</v>
       </c>
-      <c r="C81" s="95" t="s">
+      <c r="C81" s="85" t="s">
         <v>281</v>
       </c>
       <c r="D81" s="20" t="s">
@@ -6675,22 +6994,22 @@
       <c r="L81" s="48">
         <v>1</v>
       </c>
-      <c r="M81" s="96" t="s">
+      <c r="M81" s="86" t="s">
         <v>137</v>
       </c>
       <c r="N81" s="20">
         <v>-27</v>
       </c>
-      <c r="O81" s="98" t="s">
+      <c r="O81" s="88" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" s="94"/>
-      <c r="B82" s="92" t="s">
+      <c r="A82" s="84"/>
+      <c r="B82" s="83" t="s">
         <v>249</v>
       </c>
-      <c r="C82" s="95" t="s">
+      <c r="C82" s="85" t="s">
         <v>282</v>
       </c>
       <c r="D82" s="20" t="s">
@@ -6716,22 +7035,22 @@
       <c r="L82" s="48">
         <v>1</v>
       </c>
-      <c r="M82" s="96" t="s">
+      <c r="M82" s="86" t="s">
         <v>212</v>
       </c>
       <c r="N82" s="20">
         <v>-36</v>
       </c>
-      <c r="O82" s="98" t="s">
+      <c r="O82" s="88" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A83" s="94"/>
-      <c r="B83" s="92" t="s">
+      <c r="A83" s="84"/>
+      <c r="B83" s="83" t="s">
         <v>250</v>
       </c>
-      <c r="C83" s="95" t="s">
+      <c r="C83" s="85" t="s">
         <v>284</v>
       </c>
       <c r="D83" s="20" t="s">
@@ -6757,22 +7076,22 @@
       <c r="L83" s="48">
         <v>1</v>
       </c>
-      <c r="M83" s="96" t="s">
+      <c r="M83" s="86" t="s">
         <v>301</v>
       </c>
       <c r="N83" s="20">
         <v>-34</v>
       </c>
-      <c r="O83" s="98" t="s">
+      <c r="O83" s="88" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A84" s="94"/>
-      <c r="B84" s="92" t="s">
+      <c r="A84" s="84"/>
+      <c r="B84" s="83" t="s">
         <v>251</v>
       </c>
-      <c r="C84" s="95" t="s">
+      <c r="C84" s="85" t="s">
         <v>283</v>
       </c>
       <c r="D84" s="20" t="s">
@@ -6798,22 +7117,22 @@
       <c r="L84" s="48">
         <v>1</v>
       </c>
-      <c r="M84" s="96" t="s">
+      <c r="M84" s="86" t="s">
         <v>212</v>
       </c>
       <c r="N84" s="20">
         <v>-36</v>
       </c>
-      <c r="O84" s="98" t="s">
+      <c r="O84" s="88" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A85" s="94"/>
-      <c r="B85" s="92" t="s">
+      <c r="A85" s="84"/>
+      <c r="B85" s="83" t="s">
         <v>252</v>
       </c>
-      <c r="C85" s="95" t="s">
+      <c r="C85" s="85" t="s">
         <v>285</v>
       </c>
       <c r="D85" s="20" t="s">
@@ -6839,22 +7158,22 @@
       <c r="L85" s="48">
         <v>1</v>
       </c>
-      <c r="M85" s="96" t="s">
+      <c r="M85" s="86" t="s">
         <v>301</v>
       </c>
       <c r="N85" s="20">
         <v>-34</v>
       </c>
-      <c r="O85" s="98" t="s">
+      <c r="O85" s="88" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A86" s="94"/>
-      <c r="B86" s="92" t="s">
+      <c r="A86" s="84"/>
+      <c r="B86" s="83" t="s">
         <v>253</v>
       </c>
-      <c r="C86" s="95" t="s">
+      <c r="C86" s="85" t="s">
         <v>286</v>
       </c>
       <c r="D86" s="20" t="s">
@@ -6880,22 +7199,22 @@
       <c r="L86" s="48">
         <v>1</v>
       </c>
-      <c r="M86" s="96" t="s">
+      <c r="M86" s="86" t="s">
         <v>302</v>
       </c>
       <c r="N86" s="20">
         <v>-29</v>
       </c>
-      <c r="O86" s="98" t="s">
+      <c r="O86" s="88" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A87" s="94"/>
-      <c r="B87" s="92" t="s">
+      <c r="A87" s="84"/>
+      <c r="B87" s="83" t="s">
         <v>303</v>
       </c>
-      <c r="C87" s="95" t="s">
+      <c r="C87" s="85" t="s">
         <v>287</v>
       </c>
       <c r="D87" s="20" t="s">
@@ -6921,22 +7240,22 @@
       <c r="L87" s="48">
         <v>1</v>
       </c>
-      <c r="M87" s="96" t="s">
+      <c r="M87" s="86" t="s">
         <v>304</v>
       </c>
       <c r="N87" s="20">
         <v>-29</v>
       </c>
-      <c r="O87" s="98" t="s">
+      <c r="O87" s="88" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A88" s="94"/>
-      <c r="B88" s="92" t="s">
+      <c r="A88" s="84"/>
+      <c r="B88" s="83" t="s">
         <v>254</v>
       </c>
-      <c r="C88" s="95" t="s">
+      <c r="C88" s="85" t="s">
         <v>288</v>
       </c>
       <c r="D88" s="20" t="s">
@@ -6962,22 +7281,22 @@
       <c r="L88" s="48">
         <v>1</v>
       </c>
-      <c r="M88" s="96" t="s">
+      <c r="M88" s="86" t="s">
         <v>305</v>
       </c>
       <c r="N88" s="20">
         <v>-28</v>
       </c>
-      <c r="O88" s="98" t="s">
+      <c r="O88" s="88" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A89" s="94"/>
-      <c r="B89" s="92" t="s">
+      <c r="A89" s="84"/>
+      <c r="B89" s="83" t="s">
         <v>255</v>
       </c>
-      <c r="C89" s="95" t="s">
+      <c r="C89" s="85" t="s">
         <v>289</v>
       </c>
       <c r="D89" s="20" t="s">
@@ -7003,22 +7322,22 @@
       <c r="L89" s="48">
         <v>1</v>
       </c>
-      <c r="M89" s="96" t="s">
+      <c r="M89" s="86" t="s">
         <v>306</v>
       </c>
       <c r="N89" s="20">
         <v>-32</v>
       </c>
-      <c r="O89" s="98" t="s">
+      <c r="O89" s="88" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A90" s="94"/>
-      <c r="B90" s="92" t="s">
+      <c r="A90" s="84"/>
+      <c r="B90" s="83" t="s">
         <v>262</v>
       </c>
-      <c r="C90" s="95" t="s">
+      <c r="C90" s="85" t="s">
         <v>290</v>
       </c>
       <c r="D90" s="20" t="s">
@@ -7044,22 +7363,22 @@
       <c r="L90" s="48">
         <v>1</v>
       </c>
-      <c r="M90" s="96" t="s">
+      <c r="M90" s="86" t="s">
         <v>305</v>
       </c>
       <c r="N90" s="20">
         <v>-28</v>
       </c>
-      <c r="O90" s="98" t="s">
+      <c r="O90" s="88" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A91" s="94"/>
-      <c r="B91" s="92" t="s">
+      <c r="A91" s="84"/>
+      <c r="B91" s="83" t="s">
         <v>256</v>
       </c>
-      <c r="C91" s="95" t="s">
+      <c r="C91" s="85" t="s">
         <v>291</v>
       </c>
       <c r="D91" s="20" t="s">
@@ -7085,22 +7404,22 @@
       <c r="L91" s="48">
         <v>1</v>
       </c>
-      <c r="M91" s="96" t="s">
+      <c r="M91" s="86" t="s">
         <v>307</v>
       </c>
       <c r="N91" s="20">
         <v>-23</v>
       </c>
-      <c r="O91" s="98" t="s">
+      <c r="O91" s="88" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A92" s="94"/>
-      <c r="B92" s="92" t="s">
+      <c r="A92" s="84"/>
+      <c r="B92" s="83" t="s">
         <v>257</v>
       </c>
-      <c r="C92" s="95" t="s">
+      <c r="C92" s="85" t="s">
         <v>293</v>
       </c>
       <c r="D92" s="20" t="s">
@@ -7126,22 +7445,22 @@
       <c r="L92" s="48">
         <v>1</v>
       </c>
-      <c r="M92" s="96" t="s">
+      <c r="M92" s="86" t="s">
         <v>300</v>
       </c>
       <c r="N92" s="20">
         <v>-25</v>
       </c>
-      <c r="O92" s="98" t="s">
+      <c r="O92" s="88" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A93" s="94"/>
-      <c r="B93" s="92" t="s">
+      <c r="A93" s="84"/>
+      <c r="B93" s="83" t="s">
         <v>258</v>
       </c>
-      <c r="C93" s="95" t="s">
+      <c r="C93" s="85" t="s">
         <v>294</v>
       </c>
       <c r="D93" s="20" t="s">
@@ -7167,22 +7486,22 @@
       <c r="L93" s="48">
         <v>1</v>
       </c>
-      <c r="M93" s="96" t="s">
+      <c r="M93" s="86" t="s">
         <v>213</v>
       </c>
       <c r="N93" s="20">
         <v>-23</v>
       </c>
-      <c r="O93" s="98" t="s">
+      <c r="O93" s="88" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A94" s="94"/>
-      <c r="B94" s="92" t="s">
+      <c r="A94" s="84"/>
+      <c r="B94" s="83" t="s">
         <v>259</v>
       </c>
-      <c r="C94" s="95" t="s">
+      <c r="C94" s="85" t="s">
         <v>292</v>
       </c>
       <c r="D94" s="20" t="s">
@@ -7208,22 +7527,22 @@
       <c r="L94" s="48">
         <v>1</v>
       </c>
-      <c r="M94" s="96" t="s">
+      <c r="M94" s="86" t="s">
         <v>307</v>
       </c>
       <c r="N94" s="20">
         <v>-23</v>
       </c>
-      <c r="O94" s="98" t="s">
+      <c r="O94" s="88" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A95" s="94"/>
-      <c r="B95" s="92" t="s">
+      <c r="A95" s="84"/>
+      <c r="B95" s="83" t="s">
         <v>260</v>
       </c>
-      <c r="C95" s="95" t="s">
+      <c r="C95" s="85" t="s">
         <v>295</v>
       </c>
       <c r="D95" s="20" t="s">
@@ -7249,22 +7568,22 @@
       <c r="L95" s="48">
         <v>1</v>
       </c>
-      <c r="M95" s="96" t="s">
+      <c r="M95" s="86" t="s">
         <v>300</v>
       </c>
       <c r="N95" s="20">
         <v>-25</v>
       </c>
-      <c r="O95" s="98" t="s">
+      <c r="O95" s="88" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A96" s="94"/>
-      <c r="B96" s="92" t="s">
+      <c r="A96" s="84"/>
+      <c r="B96" s="83" t="s">
         <v>261</v>
       </c>
-      <c r="C96" s="95" t="s">
+      <c r="C96" s="85" t="s">
         <v>296</v>
       </c>
       <c r="D96" s="20" t="s">
@@ -7290,417 +7609,1239 @@
       <c r="L96" s="48">
         <v>1</v>
       </c>
-      <c r="M96" s="96" t="s">
+      <c r="M96" s="86" t="s">
         <v>213</v>
       </c>
       <c r="N96" s="20">
         <v>-23</v>
       </c>
-      <c r="O96" s="98" t="s">
+      <c r="O96" s="88" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A97" s="94"/>
-      <c r="B97" s="92"/>
-      <c r="C97" s="95"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="23"/>
-      <c r="F97" s="20"/>
-      <c r="G97" s="63"/>
-      <c r="H97" s="63"/>
-      <c r="I97" s="20"/>
-      <c r="J97" s="47"/>
-      <c r="K97" s="48"/>
-      <c r="L97" s="48"/>
-      <c r="M97" s="96"/>
-      <c r="N97" s="20"/>
-      <c r="O97" s="98"/>
+      <c r="A97" s="84"/>
+      <c r="B97" s="97" t="s">
+        <v>317</v>
+      </c>
+      <c r="C97" s="95" t="s">
+        <v>318</v>
+      </c>
+      <c r="D97" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E97" s="92"/>
+      <c r="F97" s="92"/>
+      <c r="G97" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H97" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I97" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J97" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K97" s="94">
+        <v>16</v>
+      </c>
+      <c r="L97" s="94">
+        <v>1</v>
+      </c>
+      <c r="M97" s="96" t="s">
+        <v>382</v>
+      </c>
+      <c r="N97" s="92">
+        <v>-36</v>
+      </c>
+      <c r="O97" s="88" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A98" s="94"/>
-      <c r="B98" s="92"/>
-      <c r="C98" s="95"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="23"/>
-      <c r="F98" s="20"/>
-      <c r="G98" s="63"/>
-      <c r="H98" s="63"/>
-      <c r="I98" s="20"/>
-      <c r="J98" s="47"/>
-      <c r="K98" s="48"/>
-      <c r="L98" s="48"/>
-      <c r="M98" s="96"/>
-      <c r="N98" s="20"/>
-      <c r="O98" s="98"/>
+      <c r="A98" s="84"/>
+      <c r="B98" s="97" t="s">
+        <v>321</v>
+      </c>
+      <c r="C98" s="95" t="s">
+        <v>322</v>
+      </c>
+      <c r="D98" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E98" s="92"/>
+      <c r="F98" s="92"/>
+      <c r="G98" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H98" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I98" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J98" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K98" s="94">
+        <v>16</v>
+      </c>
+      <c r="L98" s="94">
+        <v>1</v>
+      </c>
+      <c r="M98" s="96" t="s">
+        <v>383</v>
+      </c>
+      <c r="N98" s="92">
+        <v>-55</v>
+      </c>
+      <c r="O98" s="88" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A99" s="94"/>
-      <c r="B99" s="92"/>
-      <c r="C99" s="95"/>
-      <c r="D99" s="20"/>
-      <c r="E99" s="23"/>
-      <c r="F99" s="20"/>
-      <c r="G99" s="63"/>
-      <c r="H99" s="63"/>
-      <c r="I99" s="20"/>
-      <c r="J99" s="47"/>
-      <c r="K99" s="48"/>
-      <c r="L99" s="48"/>
-      <c r="M99" s="96"/>
-      <c r="N99" s="20"/>
-      <c r="O99" s="98"/>
+      <c r="A99" s="84"/>
+      <c r="B99" s="97" t="s">
+        <v>323</v>
+      </c>
+      <c r="C99" s="95" t="s">
+        <v>324</v>
+      </c>
+      <c r="D99" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E99" s="92"/>
+      <c r="F99" s="92"/>
+      <c r="G99" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H99" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I99" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J99" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K99" s="94">
+        <v>16</v>
+      </c>
+      <c r="L99" s="94">
+        <v>1</v>
+      </c>
+      <c r="M99" s="96" t="s">
+        <v>381</v>
+      </c>
+      <c r="N99" s="92">
+        <v>-39</v>
+      </c>
+      <c r="O99" s="88" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A100" s="94"/>
-      <c r="B100" s="92"/>
-      <c r="C100" s="95"/>
-      <c r="D100" s="20"/>
-      <c r="E100" s="23"/>
-      <c r="F100" s="20"/>
-      <c r="G100" s="63"/>
-      <c r="H100" s="63"/>
-      <c r="I100" s="20"/>
-      <c r="J100" s="47"/>
-      <c r="K100" s="48"/>
-      <c r="L100" s="48"/>
-      <c r="M100" s="96"/>
-      <c r="N100" s="20"/>
-      <c r="O100" s="98"/>
+      <c r="A100" s="84"/>
+      <c r="B100" s="97" t="s">
+        <v>325</v>
+      </c>
+      <c r="C100" s="95" t="s">
+        <v>326</v>
+      </c>
+      <c r="D100" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" s="92"/>
+      <c r="F100" s="92"/>
+      <c r="G100" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H100" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I100" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J100" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K100" s="94">
+        <v>16</v>
+      </c>
+      <c r="L100" s="94">
+        <v>1</v>
+      </c>
+      <c r="M100" s="96" t="s">
+        <v>384</v>
+      </c>
+      <c r="N100" s="92">
+        <v>-58</v>
+      </c>
+      <c r="O100" s="88" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A101" s="94"/>
-      <c r="B101" s="92"/>
-      <c r="C101" s="95"/>
-      <c r="D101" s="20"/>
-      <c r="E101" s="23"/>
-      <c r="F101" s="20"/>
-      <c r="G101" s="63"/>
-      <c r="H101" s="63"/>
-      <c r="I101" s="20"/>
-      <c r="J101" s="47"/>
-      <c r="K101" s="48"/>
-      <c r="L101" s="48"/>
-      <c r="M101" s="96"/>
-      <c r="N101" s="20"/>
-      <c r="O101" s="98"/>
+      <c r="A101" s="84"/>
+      <c r="B101" s="97" t="s">
+        <v>328</v>
+      </c>
+      <c r="C101" s="95" t="s">
+        <v>329</v>
+      </c>
+      <c r="D101" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E101" s="92"/>
+      <c r="F101" s="92"/>
+      <c r="G101" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H101" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I101" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J101" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K101" s="94">
+        <v>16</v>
+      </c>
+      <c r="L101" s="94">
+        <v>1</v>
+      </c>
+      <c r="M101" s="96" t="s">
+        <v>385</v>
+      </c>
+      <c r="N101" s="92">
+        <v>-32</v>
+      </c>
+      <c r="O101" s="88" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A102" s="94"/>
-      <c r="B102" s="92"/>
-      <c r="C102" s="95"/>
-      <c r="D102" s="20"/>
-      <c r="E102" s="23"/>
-      <c r="F102" s="20"/>
-      <c r="G102" s="63"/>
-      <c r="H102" s="63"/>
-      <c r="I102" s="20"/>
-      <c r="J102" s="47"/>
-      <c r="K102" s="48"/>
-      <c r="L102" s="48"/>
-      <c r="M102" s="96"/>
-      <c r="N102" s="20"/>
-      <c r="O102" s="98"/>
+      <c r="A102" s="84"/>
+      <c r="B102" s="97" t="s">
+        <v>330</v>
+      </c>
+      <c r="C102" s="95" t="s">
+        <v>331</v>
+      </c>
+      <c r="D102" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E102" s="92"/>
+      <c r="F102" s="92"/>
+      <c r="G102" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H102" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I102" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J102" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K102" s="94">
+        <v>16</v>
+      </c>
+      <c r="L102" s="94">
+        <v>1</v>
+      </c>
+      <c r="M102" s="96" t="s">
+        <v>386</v>
+      </c>
+      <c r="N102" s="92">
+        <v>-67</v>
+      </c>
+      <c r="O102" s="88" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A103" s="94"/>
-      <c r="B103" s="92"/>
-      <c r="C103" s="95"/>
-      <c r="D103" s="20"/>
-      <c r="E103" s="23"/>
-      <c r="F103" s="20"/>
-      <c r="G103" s="63"/>
-      <c r="H103" s="63"/>
-      <c r="I103" s="20"/>
-      <c r="J103" s="47"/>
-      <c r="K103" s="48"/>
-      <c r="L103" s="48"/>
-      <c r="M103" s="96"/>
-      <c r="N103" s="20"/>
-      <c r="O103" s="98"/>
+      <c r="A103" s="84"/>
+      <c r="B103" s="97" t="s">
+        <v>332</v>
+      </c>
+      <c r="C103" s="95" t="s">
+        <v>333</v>
+      </c>
+      <c r="D103" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E103" s="92"/>
+      <c r="F103" s="92"/>
+      <c r="G103" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H103" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I103" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J103" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K103" s="94">
+        <v>16</v>
+      </c>
+      <c r="L103" s="94">
+        <v>1</v>
+      </c>
+      <c r="M103" s="96" t="s">
+        <v>387</v>
+      </c>
+      <c r="N103" s="92">
+        <v>-38</v>
+      </c>
+      <c r="O103" s="88" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A104" s="94"/>
-      <c r="B104" s="92"/>
-      <c r="C104" s="95"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="23"/>
-      <c r="F104" s="20"/>
-      <c r="G104" s="63"/>
-      <c r="H104" s="63"/>
-      <c r="I104" s="20"/>
-      <c r="J104" s="47"/>
-      <c r="K104" s="48"/>
-      <c r="L104" s="48"/>
-      <c r="M104" s="96"/>
-      <c r="N104" s="20"/>
-      <c r="O104" s="98"/>
+      <c r="A104" s="84"/>
+      <c r="B104" s="97" t="s">
+        <v>335</v>
+      </c>
+      <c r="C104" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="D104" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E104" s="92"/>
+      <c r="F104" s="92"/>
+      <c r="G104" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H104" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I104" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J104" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K104" s="94">
+        <v>16</v>
+      </c>
+      <c r="L104" s="94">
+        <v>1</v>
+      </c>
+      <c r="M104" s="96" t="s">
+        <v>388</v>
+      </c>
+      <c r="N104" s="92">
+        <v>-73</v>
+      </c>
+      <c r="O104" s="88" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A105" s="94"/>
-      <c r="B105" s="92"/>
-      <c r="C105" s="95"/>
-      <c r="D105" s="20"/>
-      <c r="E105" s="23"/>
-      <c r="F105" s="20"/>
-      <c r="G105" s="63"/>
-      <c r="H105" s="63"/>
-      <c r="I105" s="20"/>
-      <c r="J105" s="47"/>
-      <c r="K105" s="48"/>
-      <c r="L105" s="48"/>
-      <c r="M105" s="96"/>
-      <c r="N105" s="20"/>
-      <c r="O105" s="98"/>
+      <c r="A105" s="84"/>
+      <c r="B105" s="97" t="s">
+        <v>337</v>
+      </c>
+      <c r="C105" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="D105" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E105" s="92"/>
+      <c r="F105" s="92"/>
+      <c r="G105" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H105" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I105" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J105" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K105" s="94">
+        <v>16</v>
+      </c>
+      <c r="L105" s="94">
+        <v>1</v>
+      </c>
+      <c r="M105" s="96" t="s">
+        <v>389</v>
+      </c>
+      <c r="N105" s="92">
+        <v>-43</v>
+      </c>
+      <c r="O105" s="88" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A106" s="94"/>
-      <c r="B106" s="92"/>
-      <c r="C106" s="95"/>
-      <c r="D106" s="20"/>
-      <c r="E106" s="23"/>
-      <c r="F106" s="20"/>
-      <c r="G106" s="63"/>
-      <c r="H106" s="63"/>
-      <c r="I106" s="20"/>
-      <c r="J106" s="47"/>
-      <c r="K106" s="48"/>
-      <c r="L106" s="48"/>
-      <c r="M106" s="96"/>
-      <c r="N106" s="20"/>
-      <c r="O106" s="98"/>
+      <c r="A106" s="84"/>
+      <c r="B106" s="97" t="s">
+        <v>339</v>
+      </c>
+      <c r="C106" s="95" t="s">
+        <v>340</v>
+      </c>
+      <c r="D106" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E106" s="92"/>
+      <c r="F106" s="92"/>
+      <c r="G106" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H106" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I106" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J106" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K106" s="94">
+        <v>16</v>
+      </c>
+      <c r="L106" s="94">
+        <v>1</v>
+      </c>
+      <c r="M106" s="96" t="s">
+        <v>390</v>
+      </c>
+      <c r="N106" s="92">
+        <v>-61</v>
+      </c>
+      <c r="O106" s="88" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A107" s="94"/>
-      <c r="B107" s="92"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="23"/>
-      <c r="E107" s="23"/>
-      <c r="F107" s="20"/>
-      <c r="G107" s="91"/>
-      <c r="H107" s="7"/>
-      <c r="I107" s="20"/>
-      <c r="J107" s="47"/>
-      <c r="K107" s="48"/>
-      <c r="L107" s="48"/>
-      <c r="M107" s="8"/>
-      <c r="N107" s="7"/>
-      <c r="O107" s="94"/>
+      <c r="A107" s="84"/>
+      <c r="B107" s="97" t="s">
+        <v>341</v>
+      </c>
+      <c r="C107" s="95" t="s">
+        <v>342</v>
+      </c>
+      <c r="D107" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E107" s="92"/>
+      <c r="F107" s="92"/>
+      <c r="G107" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H107" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I107" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J107" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K107" s="94">
+        <v>16</v>
+      </c>
+      <c r="L107" s="94">
+        <v>1</v>
+      </c>
+      <c r="M107" s="96" t="s">
+        <v>391</v>
+      </c>
+      <c r="N107" s="92">
+        <v>-61</v>
+      </c>
+      <c r="O107" s="88" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" s="94"/>
-      <c r="B108" s="92"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="23"/>
-      <c r="E108" s="23"/>
-      <c r="F108" s="20"/>
-      <c r="G108" s="91"/>
-      <c r="H108" s="7"/>
-      <c r="I108" s="20"/>
-      <c r="J108" s="47"/>
-      <c r="K108" s="48"/>
-      <c r="L108" s="48"/>
-      <c r="M108" s="8"/>
-      <c r="N108" s="7"/>
-      <c r="O108" s="94"/>
+      <c r="A108" s="84"/>
+      <c r="B108" s="97" t="s">
+        <v>344</v>
+      </c>
+      <c r="C108" s="95" t="s">
+        <v>345</v>
+      </c>
+      <c r="D108" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E108" s="92"/>
+      <c r="F108" s="92"/>
+      <c r="G108" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H108" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I108" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J108" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K108" s="94">
+        <v>16</v>
+      </c>
+      <c r="L108" s="94">
+        <v>1</v>
+      </c>
+      <c r="M108" s="96" t="s">
+        <v>392</v>
+      </c>
+      <c r="N108" s="92">
+        <v>-58</v>
+      </c>
+      <c r="O108" s="88" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A109" s="94"/>
-      <c r="B109" s="92"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="23"/>
-      <c r="E109" s="23"/>
-      <c r="F109" s="20"/>
-      <c r="G109" s="91"/>
-      <c r="H109" s="7"/>
-      <c r="I109" s="20"/>
-      <c r="J109" s="47"/>
-      <c r="K109" s="48"/>
-      <c r="L109" s="48"/>
-      <c r="M109" s="8"/>
-      <c r="N109" s="7"/>
-      <c r="O109" s="94"/>
+      <c r="A109" s="84"/>
+      <c r="B109" s="97" t="s">
+        <v>346</v>
+      </c>
+      <c r="C109" s="95" t="s">
+        <v>347</v>
+      </c>
+      <c r="D109" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="92"/>
+      <c r="F109" s="92"/>
+      <c r="G109" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H109" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I109" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J109" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K109" s="94">
+        <v>16</v>
+      </c>
+      <c r="L109" s="94">
+        <v>1</v>
+      </c>
+      <c r="M109" s="96" t="s">
+        <v>391</v>
+      </c>
+      <c r="N109" s="92">
+        <v>-61</v>
+      </c>
+      <c r="O109" s="88" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A110" s="94"/>
-      <c r="B110" s="92"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="23"/>
-      <c r="E110" s="23"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="91"/>
-      <c r="H110" s="7"/>
-      <c r="I110" s="20"/>
-      <c r="J110" s="47"/>
-      <c r="K110" s="48"/>
-      <c r="L110" s="48"/>
-      <c r="M110" s="8"/>
-      <c r="N110" s="7"/>
-      <c r="O110" s="94"/>
+      <c r="A110" s="84"/>
+      <c r="B110" s="97" t="s">
+        <v>348</v>
+      </c>
+      <c r="C110" s="95" t="s">
+        <v>349</v>
+      </c>
+      <c r="D110" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E110" s="92"/>
+      <c r="F110" s="92"/>
+      <c r="G110" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H110" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I110" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J110" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K110" s="94">
+        <v>16</v>
+      </c>
+      <c r="L110" s="94">
+        <v>1</v>
+      </c>
+      <c r="M110" s="96" t="s">
+        <v>393</v>
+      </c>
+      <c r="N110" s="92">
+        <v>-51</v>
+      </c>
+      <c r="O110" s="88" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A111" s="94"/>
-      <c r="B111" s="92"/>
-      <c r="C111" s="7"/>
-      <c r="D111" s="23"/>
-      <c r="E111" s="23"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="91"/>
-      <c r="H111" s="7"/>
-      <c r="I111" s="20"/>
-      <c r="J111" s="47"/>
-      <c r="K111" s="48"/>
-      <c r="L111" s="48"/>
-      <c r="M111" s="8"/>
-      <c r="N111" s="7"/>
-      <c r="O111" s="94"/>
+      <c r="A111" s="84"/>
+      <c r="B111" s="97" t="s">
+        <v>351</v>
+      </c>
+      <c r="C111" s="95" t="s">
+        <v>352</v>
+      </c>
+      <c r="D111" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E111" s="92"/>
+      <c r="F111" s="92"/>
+      <c r="G111" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H111" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I111" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J111" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K111" s="94">
+        <v>16</v>
+      </c>
+      <c r="L111" s="94">
+        <v>1</v>
+      </c>
+      <c r="M111" s="96" t="s">
+        <v>394</v>
+      </c>
+      <c r="N111" s="92">
+        <v>-55</v>
+      </c>
+      <c r="O111" s="88" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A112" s="94"/>
-      <c r="B112" s="92"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="23"/>
-      <c r="E112" s="23"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="91"/>
-      <c r="H112" s="7"/>
-      <c r="I112" s="20"/>
-      <c r="J112" s="47"/>
-      <c r="K112" s="48"/>
-      <c r="L112" s="48"/>
-      <c r="M112" s="8"/>
-      <c r="N112" s="7"/>
-      <c r="O112" s="94"/>
+      <c r="A112" s="84"/>
+      <c r="B112" s="97" t="s">
+        <v>353</v>
+      </c>
+      <c r="C112" s="95" t="s">
+        <v>354</v>
+      </c>
+      <c r="D112" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E112" s="92"/>
+      <c r="F112" s="92"/>
+      <c r="G112" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H112" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I112" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J112" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K112" s="94">
+        <v>16</v>
+      </c>
+      <c r="L112" s="94">
+        <v>1</v>
+      </c>
+      <c r="M112" s="96" t="s">
+        <v>395</v>
+      </c>
+      <c r="N112" s="92">
+        <v>-75</v>
+      </c>
+      <c r="O112" s="88" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A113" s="94"/>
-      <c r="B113" s="92"/>
-      <c r="C113" s="7"/>
-      <c r="D113" s="23"/>
-      <c r="E113" s="23"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="91"/>
-      <c r="H113" s="7"/>
-      <c r="I113" s="20"/>
-      <c r="J113" s="47"/>
-      <c r="K113" s="48"/>
-      <c r="L113" s="48"/>
-      <c r="M113" s="8"/>
-      <c r="N113" s="7"/>
-      <c r="O113" s="94"/>
+      <c r="A113" s="84"/>
+      <c r="B113" s="97" t="s">
+        <v>355</v>
+      </c>
+      <c r="C113" s="95" t="s">
+        <v>356</v>
+      </c>
+      <c r="D113" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E113" s="92"/>
+      <c r="F113" s="92"/>
+      <c r="G113" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H113" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I113" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J113" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K113" s="94">
+        <v>16</v>
+      </c>
+      <c r="L113" s="94">
+        <v>1</v>
+      </c>
+      <c r="M113" s="96" t="s">
+        <v>396</v>
+      </c>
+      <c r="N113" s="92">
+        <v>-38</v>
+      </c>
+      <c r="O113" s="88" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="94"/>
-      <c r="B114" s="92"/>
-      <c r="C114" s="7"/>
-      <c r="D114" s="23"/>
-      <c r="E114" s="23"/>
-      <c r="F114" s="20"/>
-      <c r="G114" s="91"/>
-      <c r="H114" s="7"/>
-      <c r="I114" s="20"/>
-      <c r="J114" s="47"/>
-      <c r="K114" s="48"/>
-      <c r="L114" s="48"/>
-      <c r="M114" s="8"/>
-      <c r="N114" s="7"/>
-      <c r="O114" s="94"/>
-    </row>
-    <row r="115" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="94"/>
-      <c r="B115" s="93"/>
-      <c r="C115" s="82"/>
-      <c r="D115" s="83"/>
-      <c r="E115" s="83"/>
-      <c r="F115" s="84"/>
-      <c r="G115" s="85"/>
-      <c r="H115" s="85"/>
-      <c r="I115" s="86"/>
-      <c r="J115" s="87"/>
-      <c r="K115" s="88"/>
-      <c r="L115" s="88"/>
-      <c r="M115" s="87"/>
-      <c r="N115" s="87"/>
-      <c r="O115" s="89"/>
-    </row>
-    <row r="116" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D116" s="19">
-        <f>COUNTA(D4:D115)</f>
-        <v>93</v>
-      </c>
-      <c r="E116" s="19">
-        <f>COUNTA(E4:E115)</f>
+      <c r="A114" s="84"/>
+      <c r="B114" s="97" t="s">
+        <v>357</v>
+      </c>
+      <c r="C114" s="95" t="s">
+        <v>358</v>
+      </c>
+      <c r="D114" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E114" s="92"/>
+      <c r="F114" s="92"/>
+      <c r="G114" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H114" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I114" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J114" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K114" s="94">
+        <v>16</v>
+      </c>
+      <c r="L114" s="94">
+        <v>1</v>
+      </c>
+      <c r="M114" s="96" t="s">
+        <v>397</v>
+      </c>
+      <c r="N114" s="92">
+        <v>-65</v>
+      </c>
+      <c r="O114" s="88" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A115" s="84"/>
+      <c r="B115" s="97" t="s">
+        <v>360</v>
+      </c>
+      <c r="C115" s="95" t="s">
+        <v>361</v>
+      </c>
+      <c r="D115" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E115" s="92"/>
+      <c r="F115" s="92"/>
+      <c r="G115" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H115" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I115" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J115" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K115" s="94">
+        <v>16</v>
+      </c>
+      <c r="L115" s="94">
+        <v>1</v>
+      </c>
+      <c r="M115" s="96" t="s">
+        <v>398</v>
+      </c>
+      <c r="N115" s="92">
+        <v>-43</v>
+      </c>
+      <c r="O115" s="88" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B116" s="103" t="s">
+        <v>362</v>
+      </c>
+      <c r="C116" s="95" t="s">
+        <v>363</v>
+      </c>
+      <c r="D116" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E116" s="92"/>
+      <c r="F116" s="92"/>
+      <c r="G116" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H116" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I116" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J116" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K116" s="94">
+        <v>16</v>
+      </c>
+      <c r="L116" s="94">
+        <v>1</v>
+      </c>
+      <c r="M116" s="96" t="s">
+        <v>397</v>
+      </c>
+      <c r="N116" s="92">
+        <v>-65</v>
+      </c>
+      <c r="O116" s="88" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B117" s="103" t="s">
+        <v>364</v>
+      </c>
+      <c r="C117" s="95" t="s">
+        <v>365</v>
+      </c>
+      <c r="D117" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E117" s="92"/>
+      <c r="F117" s="92"/>
+      <c r="G117" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H117" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I117" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J117" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K117" s="94">
+        <v>16</v>
+      </c>
+      <c r="L117" s="94">
+        <v>1</v>
+      </c>
+      <c r="M117" s="96" t="s">
+        <v>398</v>
+      </c>
+      <c r="N117" s="92">
+        <v>-43</v>
+      </c>
+      <c r="O117" s="88" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B118" s="103" t="s">
+        <v>366</v>
+      </c>
+      <c r="C118" s="95" t="s">
+        <v>367</v>
+      </c>
+      <c r="D118" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E118" s="92"/>
+      <c r="F118" s="92"/>
+      <c r="G118" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H118" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I118" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J118" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K118" s="94">
+        <v>16</v>
+      </c>
+      <c r="L118" s="94">
+        <v>1</v>
+      </c>
+      <c r="M118" s="105" t="s">
+        <v>399</v>
+      </c>
+      <c r="N118" s="106">
+        <v>-50</v>
+      </c>
+      <c r="O118" s="88" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B119" s="103" t="s">
+        <v>369</v>
+      </c>
+      <c r="C119" s="95" t="s">
+        <v>370</v>
+      </c>
+      <c r="D119" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E119" s="92"/>
+      <c r="F119" s="92"/>
+      <c r="G119" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H119" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I119" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J119" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K119" s="94">
+        <v>16</v>
+      </c>
+      <c r="L119" s="94">
+        <v>1</v>
+      </c>
+      <c r="M119" s="107" t="s">
+        <v>400</v>
+      </c>
+      <c r="N119" s="92">
+        <v>-36</v>
+      </c>
+      <c r="O119" s="88" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B120" s="103" t="s">
+        <v>371</v>
+      </c>
+      <c r="C120" s="95" t="s">
+        <v>372</v>
+      </c>
+      <c r="D120" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E120" s="92"/>
+      <c r="F120" s="92"/>
+      <c r="G120" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H120" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I120" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J120" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K120" s="94">
+        <v>16</v>
+      </c>
+      <c r="L120" s="94">
+        <v>1</v>
+      </c>
+      <c r="M120" s="107" t="s">
+        <v>401</v>
+      </c>
+      <c r="N120" s="92">
+        <v>-75</v>
+      </c>
+      <c r="O120" s="88" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B121" s="103" t="s">
+        <v>374</v>
+      </c>
+      <c r="C121" s="95" t="s">
+        <v>375</v>
+      </c>
+      <c r="D121" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E121" s="92"/>
+      <c r="F121" s="92"/>
+      <c r="G121" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H121" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I121" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J121" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K121" s="94">
+        <v>16</v>
+      </c>
+      <c r="L121" s="94">
+        <v>1</v>
+      </c>
+      <c r="M121" s="107" t="s">
+        <v>401</v>
+      </c>
+      <c r="N121" s="92">
+        <v>-75</v>
+      </c>
+      <c r="O121" s="88" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B122" s="103" t="s">
+        <v>376</v>
+      </c>
+      <c r="C122" s="95" t="s">
+        <v>377</v>
+      </c>
+      <c r="D122" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E122" s="92"/>
+      <c r="F122" s="92"/>
+      <c r="G122" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H122" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I122" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J122" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K122" s="94">
+        <v>16</v>
+      </c>
+      <c r="L122" s="94">
+        <v>1</v>
+      </c>
+      <c r="M122" s="107"/>
+      <c r="N122" s="92"/>
+      <c r="O122" s="88" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B123" s="103" t="s">
+        <v>379</v>
+      </c>
+      <c r="C123" s="95" t="s">
+        <v>380</v>
+      </c>
+      <c r="D123" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E123" s="92"/>
+      <c r="F123" s="92"/>
+      <c r="G123" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="H123" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="I123" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="J123" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="K123" s="94">
+        <v>16</v>
+      </c>
+      <c r="L123" s="94">
+        <v>1</v>
+      </c>
+      <c r="M123" s="107"/>
+      <c r="N123" s="92"/>
+      <c r="O123" s="88" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B124" s="104"/>
+      <c r="C124" s="98"/>
+      <c r="D124" s="99"/>
+      <c r="E124" s="99"/>
+      <c r="F124" s="99"/>
+      <c r="G124" s="100"/>
+      <c r="H124" s="100"/>
+      <c r="I124" s="99"/>
+      <c r="J124" s="101"/>
+      <c r="K124" s="101"/>
+      <c r="L124" s="101"/>
+      <c r="M124" s="101"/>
+      <c r="N124" s="101"/>
+      <c r="O124" s="102"/>
+    </row>
+    <row r="125" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="89"/>
+      <c r="C125" s="89"/>
+      <c r="D125" s="90">
+        <v>120</v>
+      </c>
+      <c r="E125" s="90">
         <v>0</v>
       </c>
-      <c r="F116" s="19">
-        <f>COUNTA(F4:F115)</f>
+      <c r="F125" s="90">
         <v>0</v>
       </c>
+      <c r="G125" s="89"/>
+      <c r="H125" s="89"/>
+      <c r="I125" s="89"/>
+      <c r="J125" s="89"/>
+      <c r="K125" s="89"/>
+      <c r="L125" s="89"/>
+      <c r="M125" s="89"/>
+      <c r="N125" s="89"/>
+      <c r="O125" s="89"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O4" r:id="rId1" location="Personajes!B5" xr:uid="{B33A0548-9DC9-4C14-A9CD-22C80F2E32F8}"/>
-    <hyperlink ref="O6" r:id="rId2" location="Personajes!B7" xr:uid="{AD58C9C9-1670-41AA-83F7-5B71FD9CC2E9}"/>
-    <hyperlink ref="O11" r:id="rId3" location="Personajes!B12" xr:uid="{ED57B468-7A57-4D60-A5A6-6AE8E6DFD019}"/>
-    <hyperlink ref="O15" r:id="rId4" location="Personajes!B16" xr:uid="{4068CF2E-5A3C-4CDD-A258-7F94FB52FB07}"/>
-    <hyperlink ref="O19" r:id="rId5" location="Personajes!B20" xr:uid="{5D878E57-0261-49F3-977E-6A679C07F932}"/>
-    <hyperlink ref="O23" r:id="rId6" location="Personajes!B24" xr:uid="{1092A368-3190-43D9-8DEF-5165FA2AAEE8}"/>
-    <hyperlink ref="O26" r:id="rId7" location="Personajes!B27" xr:uid="{5E0479EF-B340-44D7-83EA-C25D4FDB53F3}"/>
-    <hyperlink ref="O28" r:id="rId8" location="Personajes!B29" xr:uid="{A955022D-E085-4CB7-AFFF-03984A4A21D1}"/>
-    <hyperlink ref="O30" r:id="rId9" location="Personajes!B31" xr:uid="{5754CB05-7DB5-42EA-B234-D952D2FB7E32}"/>
-    <hyperlink ref="O5" r:id="rId10" location="Personajes!B5" xr:uid="{92E80E95-78DE-4790-97E0-91F27F726277}"/>
-    <hyperlink ref="O7:O10" r:id="rId11" location="Personajes!B7" display="1.2" xr:uid="{963EEC70-ABEF-4C70-BAF0-A862F8F6C539}"/>
-    <hyperlink ref="O12:O14" r:id="rId12" location="Personajes!B12" display="1.3" xr:uid="{440E36D5-6A7E-41B8-8F40-D8A255CBAAC5}"/>
-    <hyperlink ref="O16:O18" r:id="rId13" location="Personajes!B16" display="1.4" xr:uid="{2F68302D-CEF3-4AC0-B394-1AD663FBFED4}"/>
-    <hyperlink ref="O20:O22" r:id="rId14" location="Personajes!B20" display="1.5" xr:uid="{94F81431-A88C-4AB4-8DF3-B2153F53103F}"/>
-    <hyperlink ref="O24:O25" r:id="rId15" location="Personajes!B24" display="1.6" xr:uid="{E73D9855-8AA0-445D-B8DB-90F3F811DDC5}"/>
-    <hyperlink ref="O27" r:id="rId16" location="Personajes!B27" xr:uid="{B04C2F70-42E7-44B0-B051-72C56DAE147B}"/>
-    <hyperlink ref="O29" r:id="rId17" location="Personajes!B29" xr:uid="{D2DCFD11-4ABA-44A6-926D-504AE85D63DB}"/>
-    <hyperlink ref="O31:O35" r:id="rId18" location="Personajes!B31" display="1.9" xr:uid="{7C818B1F-3C66-49A3-9BC1-56DEFB3B3EF2}"/>
-    <hyperlink ref="O35" r:id="rId19" location="Personajes!B31" xr:uid="{32180BEB-0599-47D7-B37A-E3E9F39E587F}"/>
-    <hyperlink ref="O36" r:id="rId20" location="Personajes!B37" xr:uid="{E976FB3E-BDD2-4FF5-9616-4A074EF111F8}"/>
-    <hyperlink ref="O39" r:id="rId21" location="Personajes!B40" xr:uid="{6D3A29F3-4046-4EB3-827E-6A4E36F3008C}"/>
-    <hyperlink ref="O43" r:id="rId22" location="Personajes!B44" xr:uid="{AEB25276-132E-4E32-8251-385E6DE2BDD4}"/>
-    <hyperlink ref="O46" r:id="rId23" location="Personajes!B47" xr:uid="{8232ED02-497D-4F87-9DCB-0FC0E0B337E5}"/>
-    <hyperlink ref="O50" r:id="rId24" location="Personajes!B51" xr:uid="{E82F8AEF-81D4-4195-9229-4D7045F8B1A4}"/>
-    <hyperlink ref="O52" r:id="rId25" location="Personajes!B53" xr:uid="{CBF5ECD2-755B-4691-9B30-9A6FDB379912}"/>
-    <hyperlink ref="O56" r:id="rId26" location="Personajes!B57" xr:uid="{38455E00-92AC-42EE-8682-2DFBB8B3EA90}"/>
-    <hyperlink ref="O59" r:id="rId27" location="Personajes!B60" xr:uid="{DD8F4AEA-D3E9-476C-929A-815DF1364F50}"/>
-    <hyperlink ref="O61" r:id="rId28" location="Personajes!B62" xr:uid="{BC88D34C-27FC-49E5-9EF8-57882A8948E1}"/>
-    <hyperlink ref="O37:O38" r:id="rId29" location="Personajes!B37" display="2.1" xr:uid="{7E687246-EC35-4F51-B65E-134E8FB881A8}"/>
-    <hyperlink ref="O40:O42" r:id="rId30" location="Personajes!B40" display="2.2" xr:uid="{DAB6977C-9901-4100-8AA0-A83160E6486E}"/>
-    <hyperlink ref="O44:O45" r:id="rId31" location="Personajes!B44" display="2.3" xr:uid="{ADD79FED-57AE-46BD-860F-1A1D73C84E9C}"/>
-    <hyperlink ref="O47:O49" r:id="rId32" location="Personajes!B47" display="2.4" xr:uid="{0B4C5A4C-6474-4351-995B-531DFBA6C9C9}"/>
-    <hyperlink ref="O51" r:id="rId33" location="Personajes!B51" xr:uid="{17BEAB1D-BCED-411F-80C2-50DD8954E1FB}"/>
-    <hyperlink ref="O53:O55" r:id="rId34" location="Personajes!B53" display="2.6" xr:uid="{9FD7819D-5A82-401C-932C-CA1B704E982E}"/>
-    <hyperlink ref="O57:O58" r:id="rId35" location="Personajes!B57" display="2.7" xr:uid="{B04FAF41-9941-4BF2-924F-25F1939928C0}"/>
-    <hyperlink ref="O60" r:id="rId36" location="Personajes!B60" xr:uid="{E5508906-E8BF-49D2-93B6-8000308BE4E6}"/>
-    <hyperlink ref="O62" r:id="rId37" location="Personajes!B62" xr:uid="{4D7A5D8C-B071-4453-A203-AC18BEF2C66B}"/>
-    <hyperlink ref="O63" r:id="rId38" location="Personajes!B64" xr:uid="{C6ED0C5D-A122-4F7D-84A1-283B76B6F9AE}"/>
-    <hyperlink ref="O65" r:id="rId39" location="Personajes!B66" xr:uid="{D3A5A1E5-A122-4885-80A2-85DCC72DB805}"/>
-    <hyperlink ref="O69" r:id="rId40" location="Personajes!B70" xr:uid="{DA3ED20A-0D4F-4E9B-B012-E795FBF05D82}"/>
-    <hyperlink ref="O71" r:id="rId41" location="Personajes!B72" xr:uid="{AFE80BEF-15A8-4D7E-B578-4A7E8029BF25}"/>
-    <hyperlink ref="O76" r:id="rId42" location="Personajes!B77" xr:uid="{D84330C9-45C7-4805-B190-ED9AC4CCF420}"/>
-    <hyperlink ref="O82" r:id="rId43" location="Personajes!B83" xr:uid="{3B1320E3-4F69-4A71-B8C9-B248EC150584}"/>
-    <hyperlink ref="O86" r:id="rId44" location="Personajes!B87" xr:uid="{F11006AA-9519-45A2-88A6-8EFB43798C98}"/>
-    <hyperlink ref="O88" r:id="rId45" location="Personajes!B89" xr:uid="{1D1E7D58-1A8E-456A-BE85-FDDE537A8B1F}"/>
-    <hyperlink ref="O91" r:id="rId46" location="Personajes!B92" xr:uid="{3E93AE16-AA16-409D-9C8A-982EBFFEEAC9}"/>
-    <hyperlink ref="O64" r:id="rId47" location="Personajes!B64" xr:uid="{BD88B733-5B0D-44FB-B2FC-E74844849C9B}"/>
-    <hyperlink ref="O66:O68" r:id="rId48" location="Personajes!B66" display="3.2" xr:uid="{1FD704E4-9606-4F5E-BA37-8533362CDF22}"/>
-    <hyperlink ref="O70" r:id="rId49" location="Personajes!B70" xr:uid="{707AA539-D206-415A-B9D9-D4D4DC543C25}"/>
-    <hyperlink ref="O72:O75" r:id="rId50" location="Personajes!B72" display="3.4" xr:uid="{17DE853D-4F86-4FA4-885F-1C77FDFF750B}"/>
-    <hyperlink ref="O77:O81" r:id="rId51" location="Personajes!B77" display="3.5" xr:uid="{9C2F3363-F444-4CBA-B5DA-ADF6A21628E5}"/>
-    <hyperlink ref="O83:O85" r:id="rId52" location="Personajes!B83" display="3.6" xr:uid="{71607043-1BDA-4094-BBBE-38E341349CE1}"/>
-    <hyperlink ref="O87" r:id="rId53" location="Personajes!B87" xr:uid="{75DB7810-AFDC-43DB-8CB9-974E87F69769}"/>
-    <hyperlink ref="O89:O90" r:id="rId54" location="Personajes!B89" display="3.8" xr:uid="{21A954C3-EB34-488B-953A-F74266A8AAF8}"/>
-    <hyperlink ref="O92:O96" r:id="rId55" location="Personajes!B92" display="3.9" xr:uid="{C03D6EEB-CB77-4173-B0A8-1354D40BAB57}"/>
+    <hyperlink ref="O4" r:id="rId1" location="Personajes!B5"/>
+    <hyperlink ref="O6" r:id="rId2" location="Personajes!B7"/>
+    <hyperlink ref="O11" r:id="rId3" location="Personajes!B12"/>
+    <hyperlink ref="O15" r:id="rId4" location="Personajes!B16"/>
+    <hyperlink ref="O19" r:id="rId5" location="Personajes!B20"/>
+    <hyperlink ref="O23" r:id="rId6" location="Personajes!B24"/>
+    <hyperlink ref="O26" r:id="rId7" location="Personajes!B27"/>
+    <hyperlink ref="O28" r:id="rId8" location="Personajes!B29"/>
+    <hyperlink ref="O30" r:id="rId9" location="Personajes!B31"/>
+    <hyperlink ref="O5" r:id="rId10" location="Personajes!B5"/>
+    <hyperlink ref="O7:O10" r:id="rId11" location="Personajes!B7" display="1.2"/>
+    <hyperlink ref="O12:O14" r:id="rId12" location="Personajes!B12" display="1.3"/>
+    <hyperlink ref="O16:O18" r:id="rId13" location="Personajes!B16" display="1.4"/>
+    <hyperlink ref="O20:O22" r:id="rId14" location="Personajes!B20" display="1.5"/>
+    <hyperlink ref="O24:O25" r:id="rId15" location="Personajes!B24" display="1.6"/>
+    <hyperlink ref="O27" r:id="rId16" location="Personajes!B27"/>
+    <hyperlink ref="O29" r:id="rId17" location="Personajes!B29"/>
+    <hyperlink ref="O31:O35" r:id="rId18" location="Personajes!B31" display="1.9"/>
+    <hyperlink ref="O35" r:id="rId19" location="Personajes!B31"/>
+    <hyperlink ref="O36" r:id="rId20" location="Personajes!B37"/>
+    <hyperlink ref="O39" r:id="rId21" location="Personajes!B40"/>
+    <hyperlink ref="O43" r:id="rId22" location="Personajes!B44"/>
+    <hyperlink ref="O46" r:id="rId23" location="Personajes!B47"/>
+    <hyperlink ref="O50" r:id="rId24" location="Personajes!B51"/>
+    <hyperlink ref="O52" r:id="rId25" location="Personajes!B53"/>
+    <hyperlink ref="O56" r:id="rId26" location="Personajes!B57"/>
+    <hyperlink ref="O59" r:id="rId27" location="Personajes!B60"/>
+    <hyperlink ref="O61" r:id="rId28" location="Personajes!B62"/>
+    <hyperlink ref="O37:O38" r:id="rId29" location="Personajes!B37" display="2.1"/>
+    <hyperlink ref="O40:O42" r:id="rId30" location="Personajes!B40" display="2.2"/>
+    <hyperlink ref="O44:O45" r:id="rId31" location="Personajes!B44" display="2.3"/>
+    <hyperlink ref="O47:O49" r:id="rId32" location="Personajes!B47" display="2.4"/>
+    <hyperlink ref="O51" r:id="rId33" location="Personajes!B51"/>
+    <hyperlink ref="O53:O55" r:id="rId34" location="Personajes!B53" display="2.6"/>
+    <hyperlink ref="O57:O58" r:id="rId35" location="Personajes!B57" display="2.7"/>
+    <hyperlink ref="O60" r:id="rId36" location="Personajes!B60"/>
+    <hyperlink ref="O62" r:id="rId37" location="Personajes!B62"/>
+    <hyperlink ref="O63" r:id="rId38" location="Personajes!B64"/>
+    <hyperlink ref="O65" r:id="rId39" location="Personajes!B66"/>
+    <hyperlink ref="O69" r:id="rId40" location="Personajes!B70"/>
+    <hyperlink ref="O71" r:id="rId41" location="Personajes!B72"/>
+    <hyperlink ref="O76" r:id="rId42" location="Personajes!B77"/>
+    <hyperlink ref="O82" r:id="rId43" location="Personajes!B83"/>
+    <hyperlink ref="O86" r:id="rId44" location="Personajes!B87"/>
+    <hyperlink ref="O88" r:id="rId45" location="Personajes!B89"/>
+    <hyperlink ref="O91" r:id="rId46" location="Personajes!B92"/>
+    <hyperlink ref="O64" r:id="rId47" location="Personajes!B64"/>
+    <hyperlink ref="O66:O68" r:id="rId48" location="Personajes!B66" display="3.2"/>
+    <hyperlink ref="O70" r:id="rId49" location="Personajes!B70"/>
+    <hyperlink ref="O72:O75" r:id="rId50" location="Personajes!B72" display="3.4"/>
+    <hyperlink ref="O77:O81" r:id="rId51" location="Personajes!B77" display="3.5"/>
+    <hyperlink ref="O83:O85" r:id="rId52" location="Personajes!B83" display="3.6"/>
+    <hyperlink ref="O87" r:id="rId53" location="Personajes!B87"/>
+    <hyperlink ref="O89:O90" r:id="rId54" location="Personajes!B89" display="3.8"/>
+    <hyperlink ref="O92:O96" r:id="rId55" location="Personajes!B92" display="3.9"/>
+    <hyperlink ref="O97" r:id="rId56" location="Personajes!B98"/>
+    <hyperlink ref="O98" r:id="rId57" location="Personajes!B98"/>
+    <hyperlink ref="O99" r:id="rId58" location="Personajes!B98"/>
+    <hyperlink ref="O100" r:id="rId59" location="Personajes!B101"/>
+    <hyperlink ref="O101" r:id="rId60" location="Personajes!B101"/>
+    <hyperlink ref="O102" r:id="rId61" location="Personajes!B101"/>
+    <hyperlink ref="O103" r:id="rId62" location="Personajes!B104"/>
+    <hyperlink ref="O104" r:id="rId63" location="Personajes!B104"/>
+    <hyperlink ref="O105" r:id="rId64" location="Personajes!B104"/>
+    <hyperlink ref="O106" r:id="rId65" location="Personajes!B104"/>
+    <hyperlink ref="O107" r:id="rId66" location="Personajes!B108"/>
+    <hyperlink ref="O108" r:id="rId67" location="Personajes!B108"/>
+    <hyperlink ref="O109" r:id="rId68" location="Personajes!B108"/>
+    <hyperlink ref="O110" r:id="rId69" location="Personajes!B111"/>
+    <hyperlink ref="O111" r:id="rId70" location="Personajes!B111"/>
+    <hyperlink ref="O112" r:id="rId71" location="Personajes!B111"/>
+    <hyperlink ref="O113" r:id="rId72" location="Personajes!B111"/>
+    <hyperlink ref="O114" r:id="rId73" location="Personajes!B115"/>
+    <hyperlink ref="O115" r:id="rId74" location="Personajes!B115"/>
+    <hyperlink ref="O116" r:id="rId75" location="Personajes!B115"/>
+    <hyperlink ref="O117" r:id="rId76" location="Personajes!B115"/>
+    <hyperlink ref="O118" r:id="rId77" location="Personajes!B119"/>
+    <hyperlink ref="O119" r:id="rId78" location="Personajes!B119"/>
+    <hyperlink ref="O120" r:id="rId79" location="Personajes!B121"/>
+    <hyperlink ref="O121" r:id="rId80" location="Personajes!B121"/>
+    <hyperlink ref="O122" r:id="rId81" location="Personajes!B123"/>
+    <hyperlink ref="O123" r:id="rId82" location="Personajes!B123"/>
+    <hyperlink ref="O100:O102" r:id="rId83" location="Personajes!B101" display="4.2"/>
+    <hyperlink ref="O103:O106" r:id="rId84" location="Personajes!B104" display="4.3"/>
+    <hyperlink ref="O107:O109" r:id="rId85" location="Personajes!B108" display="4.4"/>
+    <hyperlink ref="O110:O113" r:id="rId86" location="Personajes!B111" display="4.5"/>
+    <hyperlink ref="O114:O117" r:id="rId87" location="Personajes!B115" display="4.6"/>
+    <hyperlink ref="O118:O119" r:id="rId88" location="Personajes!B119" display="4.7"/>
+    <hyperlink ref="O120:O121" r:id="rId89" location="Personajes!B121" display="4.8"/>
+    <hyperlink ref="O122:O123" r:id="rId90" location="Personajes!B123" display="4.9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId56"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId91"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Frases de los personajes añadidas en la cuesheet
</commit_message>
<xml_diff>
--- a/Docs/TDS/TablaMetadatos.xlsx
+++ b/Docs/TDS/TablaMetadatos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="500" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -2448,8 +2448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5015,8 +5015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O125"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actualizada tabla metadatos TDS
</commit_message>
<xml_diff>
--- a/Docs/TDS/TablaMetadatos.xlsx
+++ b/Docs/TDS/TablaMetadatos.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo-PT\Desktop\Proyectos GitHub\Wasted-Racing\Docs\TDS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
     <sheet name="Metadatos D" sheetId="6" r:id="rId6"/>
     <sheet name="Metadatos V" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="530">
   <si>
     <t>Metadatos - Global + Estadísticas</t>
   </si>
@@ -1575,6 +1570,51 @@
   </si>
   <si>
     <t>00.13.851</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/jacobzeier/sounds/166178/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/theolm/sounds/264934/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Nakhas/sounds/344817/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/magnus589/sounds/184576/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/kyles/sounds/406483/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/dobroide/sounds/65471/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/newagesoup/sounds/377827/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/karolist/sounds/370632/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Anandthethird/sounds/366750/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/j1987/sounds/140727/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/EverydaySounds/sounds/125064/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/deleted_user_7146007/sounds/383657/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/YOH/sounds/259733/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/MrAuralization/sounds/320844/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/HuvaaKoodia/sounds/77172/</t>
   </si>
 </sst>
 </file>
@@ -2107,9 +2147,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Texto explicativo" xfId="2" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2447,7 +2487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2461,7 +2501,7 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
@@ -2549,15 +2589,15 @@
         <v>8</v>
       </c>
       <c r="C8" s="8">
-        <f>'Metadatos H'!D30</f>
+        <f>'Metadatos H'!D51</f>
         <v>0</v>
       </c>
       <c r="D8" s="8">
-        <f>'Metadatos H'!E30</f>
+        <f>'Metadatos H'!E51</f>
         <v>0</v>
       </c>
       <c r="E8" s="8">
-        <f>'Metadatos H'!F30</f>
+        <f>'Metadatos H'!F51</f>
         <v>25</v>
       </c>
       <c r="F8" s="9">
@@ -2652,11 +2692,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
@@ -3140,7 +3180,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
@@ -3364,13 +3404,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView topLeftCell="H7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
@@ -4481,32 +4521,421 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="33"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="37"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="30"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="80"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D30" s="2">
-        <f>COUNTA(D4:D29)</f>
+      <c r="A30" s="45"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29" t="s">
+        <v>515</v>
+      </c>
+      <c r="H30" s="30"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="80"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="45"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="29" t="s">
+        <v>516</v>
+      </c>
+      <c r="H31" s="30"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="80"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="45"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29" t="s">
+        <v>517</v>
+      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="80"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="45"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29" t="s">
+        <v>518</v>
+      </c>
+      <c r="H33" s="30"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="80"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="45"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29" t="s">
+        <v>519</v>
+      </c>
+      <c r="H34" s="30"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="80"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="45"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="79" t="s">
+        <v>520</v>
+      </c>
+      <c r="H35" s="30"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="80"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="45"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="29" t="s">
+        <v>521</v>
+      </c>
+      <c r="H36" s="30"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="80"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="45"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="29" t="s">
+        <v>522</v>
+      </c>
+      <c r="H37" s="30"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="80"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="45"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="29" t="s">
+        <v>523</v>
+      </c>
+      <c r="H38" s="30"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="80"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="45"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="29" t="s">
+        <v>524</v>
+      </c>
+      <c r="H39" s="30"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="80"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="45"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="29" t="s">
+        <v>525</v>
+      </c>
+      <c r="H40" s="30"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="80"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="45"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="29" t="s">
+        <v>526</v>
+      </c>
+      <c r="H41" s="30"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="80"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="45"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="29" t="s">
+        <v>528</v>
+      </c>
+      <c r="H42" s="30"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="80"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="45"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="79"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="29" t="s">
+        <v>527</v>
+      </c>
+      <c r="H43" s="30"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="80"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="45"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="29" t="s">
+        <v>529</v>
+      </c>
+      <c r="H44" s="30"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="31"/>
+      <c r="O44" s="80"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="45"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="31"/>
+      <c r="K45" s="31"/>
+      <c r="L45" s="31"/>
+      <c r="M45" s="31"/>
+      <c r="N45" s="31"/>
+      <c r="O45" s="80"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="45"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="79"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="80"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="45"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="31"/>
+      <c r="O47" s="80"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="45"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="31"/>
+      <c r="O48" s="80"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="45"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="80"/>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="33"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="34"/>
+      <c r="L50" s="34"/>
+      <c r="M50" s="36"/>
+      <c r="N50" s="34"/>
+      <c r="O50" s="37"/>
+    </row>
+    <row r="51" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D51" s="2">
+        <f>COUNTA(D4:D50)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="2">
-        <f>COUNTA(E4:E29)</f>
+      <c r="E51" s="2">
+        <f>COUNTA(E4:E50)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="2">
-        <f>COUNTA(F4:F29)</f>
+      <c r="F51" s="2">
+        <f>COUNTA(F4:F50)</f>
         <v>25</v>
       </c>
     </row>
@@ -4570,6 +4999,7 @@
     <hyperlink ref="C28" r:id="rId56"/>
     <hyperlink ref="O28" r:id="rId57" location="'Niveles'!B15"/>
     <hyperlink ref="O27" r:id="rId58" location="'Niveles'!B9"/>
+    <hyperlink ref="G35" r:id="rId59"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4584,7 +5014,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
@@ -4782,11 +5212,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
@@ -5071,7 +5501,7 @@
       <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>

</xml_diff>

<commit_message>
Actualizada cuesheet con trailer
</commit_message>
<xml_diff>
--- a/Docs/TDS/TablaMetadatos.xlsx
+++ b/Docs/TDS/TablaMetadatos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo-PT\Desktop\Wasted-Racing-master\Wasted-Racing-master\Docs\TDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo-PT\Documents\GitHub\Wasted-Racing\Docs\TDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="660">
   <si>
     <t>Metadatos - Global + Estadísticas</t>
   </si>
@@ -1595,9 +1595,6 @@
     <t>https://freesound.org/people/dobroide/sounds/65471/</t>
   </si>
   <si>
-    <t>https://freesound.org/people/newagesoup/sounds/377827/</t>
-  </si>
-  <si>
     <t>https://freesound.org/people/karolist/sounds/370632/</t>
   </si>
   <si>
@@ -1794,13 +1791,249 @@
   </si>
   <si>
     <t>1.15</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/VHS_effect.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/VHS_beep.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/spray_effect.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/city_night_ambient.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/370632__karolist__slow-motion-sound.wav</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/metalic_hit_1.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/metalic_hit_2.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/fluorescent_hum.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/VHS_play.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/fluorescent_tilt.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/cyborg_eye.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/camera_noise.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/interference_first.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/interference_second.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/interference_third.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/metalic_hit.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/rollerblade_doppler.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/rollerblade_doppler_2.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/rollerblade_spinning.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/rollerblade_acceleration.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/rollerblade_acceleration_2.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/sparks.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/explosion_1.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/laces_1.mp3</t>
+  </si>
+  <si>
+    <t>Game/media/audio/credits/laces_2.mp3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Revisable en el .aup en: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="8.8000000000000007"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Docs/TDS/Credits/</t>
+    </r>
+  </si>
+  <si>
+    <t>.mp3</t>
+  </si>
+  <si>
+    <t>.wav</t>
+  </si>
+  <si>
+    <t>00.03.239</t>
+  </si>
+  <si>
+    <t>00.01.332</t>
+  </si>
+  <si>
+    <t>00.02.769</t>
+  </si>
+  <si>
+    <t>00.00.504</t>
+  </si>
+  <si>
+    <t>00.01.128</t>
+  </si>
+  <si>
+    <t>00.05.400</t>
+  </si>
+  <si>
+    <t>00.05.088</t>
+  </si>
+  <si>
+    <t>16.0</t>
+  </si>
+  <si>
+    <t>00.04.824</t>
+  </si>
+  <si>
+    <t>00.00.240</t>
+  </si>
+  <si>
+    <t>00.00.528</t>
+  </si>
+  <si>
+    <t>00.01.149</t>
+  </si>
+  <si>
+    <t>00.04.296</t>
+  </si>
+  <si>
+    <t>00.00.287</t>
+  </si>
+  <si>
+    <t>00.13.087</t>
+  </si>
+  <si>
+    <t>00.04.661</t>
+  </si>
+  <si>
+    <t>00.00.432</t>
+  </si>
+  <si>
+    <t>00.00.549</t>
+  </si>
+  <si>
+    <t>00.00.653</t>
+  </si>
+  <si>
+    <t>00.10.848</t>
+  </si>
+  <si>
+    <t>00.01.123</t>
+  </si>
+  <si>
+    <t>00.02.717</t>
+  </si>
+  <si>
+    <t>H-028</t>
+  </si>
+  <si>
+    <t>H-029</t>
+  </si>
+  <si>
+    <t>H-030</t>
+  </si>
+  <si>
+    <t>H-031</t>
+  </si>
+  <si>
+    <t>H-032</t>
+  </si>
+  <si>
+    <t>H-033</t>
+  </si>
+  <si>
+    <t>H-034</t>
+  </si>
+  <si>
+    <t>H-035</t>
+  </si>
+  <si>
+    <t>H-036</t>
+  </si>
+  <si>
+    <t>H-037</t>
+  </si>
+  <si>
+    <t>H-038</t>
+  </si>
+  <si>
+    <t>H-039</t>
+  </si>
+  <si>
+    <t>H-040</t>
+  </si>
+  <si>
+    <t>H-041</t>
+  </si>
+  <si>
+    <t>H-042</t>
+  </si>
+  <si>
+    <t>H-043</t>
+  </si>
+  <si>
+    <t>H-045</t>
+  </si>
+  <si>
+    <t>H-046</t>
+  </si>
+  <si>
+    <t>H-047</t>
+  </si>
+  <si>
+    <t>H-048</t>
+  </si>
+  <si>
+    <t>H-049</t>
+  </si>
+  <si>
+    <t>H-050</t>
+  </si>
+  <si>
+    <t>1.10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1888,6 +2121,13 @@
     </font>
     <font>
       <sz val="8.8000000000000007"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8.8000000000000007"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2163,7 +2403,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2322,6 +2562,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2674,8 +2918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2766,20 +3010,20 @@
         <v>8</v>
       </c>
       <c r="C8" s="8">
-        <f>'Metadatos H'!D50</f>
+        <f>'Metadatos H'!D62</f>
         <v>0</v>
       </c>
       <c r="D8" s="8">
-        <f>'Metadatos H'!E50</f>
+        <f>'Metadatos H'!E62</f>
         <v>0</v>
       </c>
       <c r="E8" s="8">
-        <f>'Metadatos H'!F50</f>
-        <v>42</v>
+        <f>'Metadatos H'!F62</f>
+        <v>54</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -2848,7 +3092,7 @@
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F12" s="13">
         <f>SUM(F6:F11)</f>
-        <v>188</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2870,7 +3114,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3581,17 +3825,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" customWidth="1"/>
+    <col min="3" max="3" width="57" customWidth="1"/>
     <col min="4" max="6" width="3" style="2" customWidth="1"/>
     <col min="7" max="7" width="57.85546875" customWidth="1"/>
     <col min="8" max="8" width="59.7109375" customWidth="1"/>
@@ -4699,344 +4943,667 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="45"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="76"/>
+      <c r="B29" s="26" t="s">
+        <v>654</v>
+      </c>
+      <c r="C29" s="76" t="s">
+        <v>609</v>
+      </c>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
       <c r="F29" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G29" s="76" t="s">
-        <v>101</v>
-      </c>
-      <c r="H29" s="30"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="77"/>
+      <c r="G29" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K29" s="31">
+        <v>32</v>
+      </c>
+      <c r="L29" s="31">
+        <v>2</v>
+      </c>
+      <c r="M29" s="31" t="s">
+        <v>615</v>
+      </c>
+      <c r="N29" s="31">
+        <v>0</v>
+      </c>
+      <c r="O29" s="77" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="45"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="76"/>
+      <c r="B30" s="26" t="s">
+        <v>647</v>
+      </c>
+      <c r="C30" s="76" t="s">
+        <v>610</v>
+      </c>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
       <c r="F30" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G30" s="76" t="s">
-        <v>515</v>
-      </c>
-      <c r="H30" s="30"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="77"/>
+      <c r="G30" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K30" s="31">
+        <v>32</v>
+      </c>
+      <c r="L30" s="31">
+        <v>1</v>
+      </c>
+      <c r="M30" s="31" t="s">
+        <v>616</v>
+      </c>
+      <c r="N30" s="31">
+        <v>-28.5</v>
+      </c>
+      <c r="O30" s="77" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="45"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="76"/>
+      <c r="B31" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="C31" s="76" t="s">
+        <v>611</v>
+      </c>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28" t="s">
         <v>27</v>
       </c>
       <c r="G31" s="29" t="s">
-        <v>516</v>
-      </c>
-      <c r="H31" s="30"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="77"/>
+        <v>57</v>
+      </c>
+      <c r="H31" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I31" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J31" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K31" s="31">
+        <v>32</v>
+      </c>
+      <c r="L31" s="31">
+        <v>1</v>
+      </c>
+      <c r="M31" s="31" t="s">
+        <v>617</v>
+      </c>
+      <c r="N31" s="31">
+        <v>-10</v>
+      </c>
+      <c r="O31" s="77" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="45"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="76"/>
+      <c r="B32" s="26" t="s">
+        <v>639</v>
+      </c>
+      <c r="C32" s="76" t="s">
+        <v>603</v>
+      </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="29" t="s">
-        <v>517</v>
-      </c>
-      <c r="H32" s="30"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="77"/>
+      <c r="G32" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="H32" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J32" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K32" s="31">
+        <v>32</v>
+      </c>
+      <c r="L32" s="31">
+        <v>2</v>
+      </c>
+      <c r="M32" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="N32" s="31">
+        <v>-31.5</v>
+      </c>
+      <c r="O32" s="77" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="45"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="76"/>
+      <c r="B33" s="26" t="s">
+        <v>639</v>
+      </c>
+      <c r="C33" s="76" t="s">
+        <v>604</v>
+      </c>
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
       <c r="F33" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="29" t="s">
-        <v>518</v>
-      </c>
-      <c r="H33" s="30"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
+      <c r="G33" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J33" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K33" s="31">
+        <v>32</v>
+      </c>
+      <c r="L33" s="31">
+        <v>2</v>
+      </c>
+      <c r="M33" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="N33" s="31">
+        <v>-31</v>
+      </c>
+      <c r="O33" s="77" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="45"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="76"/>
+      <c r="B34" s="26" t="s">
+        <v>655</v>
+      </c>
+      <c r="C34" s="76" t="s">
+        <v>605</v>
+      </c>
       <c r="D34" s="28"/>
       <c r="E34" s="28"/>
       <c r="F34" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G34" s="29" t="s">
-        <v>519</v>
-      </c>
-      <c r="H34" s="30"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="O34" s="77"/>
+      <c r="G34" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="H34" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I34" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J34" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K34" s="31">
+        <v>32</v>
+      </c>
+      <c r="L34" s="31">
+        <v>2</v>
+      </c>
+      <c r="M34" s="31" t="s">
+        <v>620</v>
+      </c>
+      <c r="N34" s="31">
+        <v>-5</v>
+      </c>
+      <c r="O34" s="77" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="45"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="76"/>
+      <c r="B35" s="26" t="s">
+        <v>641</v>
+      </c>
+      <c r="C35" s="76" t="s">
+        <v>598</v>
+      </c>
       <c r="D35" s="28"/>
       <c r="E35" s="28"/>
       <c r="F35" s="28" t="s">
         <v>27</v>
       </c>
       <c r="G35" s="76" t="s">
-        <v>520</v>
-      </c>
-      <c r="H35" s="30"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="77"/>
+        <v>515</v>
+      </c>
+      <c r="H35" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I35" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K35" s="31">
+        <v>32</v>
+      </c>
+      <c r="L35" s="31">
+        <v>1</v>
+      </c>
+      <c r="M35" s="31" t="s">
+        <v>621</v>
+      </c>
+      <c r="N35" s="31">
+        <v>-35</v>
+      </c>
+      <c r="O35" s="77" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="45"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="76"/>
+      <c r="B36" s="26" t="s">
+        <v>637</v>
+      </c>
+      <c r="C36" s="76" t="s">
+        <v>587</v>
+      </c>
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
       <c r="F36" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G36" s="29" t="s">
-        <v>521</v>
-      </c>
-      <c r="H36" s="30"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="77"/>
+      <c r="G36" s="76" t="s">
+        <v>515</v>
+      </c>
+      <c r="H36" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I36" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J36" s="31" t="s">
+        <v>622</v>
+      </c>
+      <c r="K36" s="31">
+        <v>32</v>
+      </c>
+      <c r="L36" s="31">
+        <v>2</v>
+      </c>
+      <c r="M36" s="31" t="s">
+        <v>623</v>
+      </c>
+      <c r="N36" s="31">
+        <v>-18</v>
+      </c>
+      <c r="O36" s="77" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="45"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="76"/>
+      <c r="B37" s="26" t="s">
+        <v>637</v>
+      </c>
+      <c r="C37" s="76" t="s">
+        <v>587</v>
+      </c>
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
       <c r="F37" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="29" t="s">
-        <v>522</v>
-      </c>
-      <c r="H37" s="30"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31"/>
-      <c r="M37" s="31"/>
-      <c r="N37" s="31"/>
-      <c r="O37" s="77"/>
+      <c r="G37" s="76" t="s">
+        <v>516</v>
+      </c>
+      <c r="H37" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I37" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J37" s="31" t="s">
+        <v>622</v>
+      </c>
+      <c r="K37" s="31">
+        <v>32</v>
+      </c>
+      <c r="L37" s="31">
+        <v>2</v>
+      </c>
+      <c r="M37" s="31" t="s">
+        <v>623</v>
+      </c>
+      <c r="N37" s="31">
+        <v>-18</v>
+      </c>
+      <c r="O37" s="77" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="45"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="76"/>
+      <c r="B38" s="26" t="s">
+        <v>640</v>
+      </c>
+      <c r="C38" s="76" t="s">
+        <v>599</v>
+      </c>
       <c r="D38" s="28"/>
       <c r="E38" s="28"/>
       <c r="F38" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G38" s="29" t="s">
-        <v>523</v>
-      </c>
-      <c r="H38" s="30"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="31"/>
-      <c r="L38" s="31"/>
-      <c r="M38" s="31"/>
-      <c r="N38" s="31"/>
-      <c r="O38" s="77"/>
+      <c r="G38" s="76" t="s">
+        <v>516</v>
+      </c>
+      <c r="H38" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I38" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J38" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K38" s="31">
+        <v>32</v>
+      </c>
+      <c r="L38" s="31">
+        <v>2</v>
+      </c>
+      <c r="M38" s="31" t="s">
+        <v>624</v>
+      </c>
+      <c r="N38" s="31">
+        <v>-5</v>
+      </c>
+      <c r="O38" s="77" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="45"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="76"/>
+      <c r="B39" s="26" t="s">
+        <v>642</v>
+      </c>
+      <c r="C39" s="76" t="s">
+        <v>600</v>
+      </c>
       <c r="D39" s="28"/>
       <c r="E39" s="28"/>
       <c r="F39" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="29" t="s">
-        <v>524</v>
-      </c>
-      <c r="H39" s="30"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="31"/>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="77"/>
+      <c r="G39" s="76" t="s">
+        <v>516</v>
+      </c>
+      <c r="H39" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I39" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K39" s="31">
+        <v>32</v>
+      </c>
+      <c r="L39" s="31">
+        <v>2</v>
+      </c>
+      <c r="M39" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="N39" s="31">
+        <v>-5</v>
+      </c>
+      <c r="O39" s="77" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="45"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="76"/>
+      <c r="B40" s="26" t="s">
+        <v>643</v>
+      </c>
+      <c r="C40" s="76" t="s">
+        <v>601</v>
+      </c>
       <c r="D40" s="28"/>
       <c r="E40" s="28"/>
       <c r="F40" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G40" s="29" t="s">
-        <v>525</v>
-      </c>
-      <c r="H40" s="30"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="77"/>
+      <c r="G40" s="76" t="s">
+        <v>516</v>
+      </c>
+      <c r="H40" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I40" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J40" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K40" s="31">
+        <v>32</v>
+      </c>
+      <c r="L40" s="31">
+        <v>2</v>
+      </c>
+      <c r="M40" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="N40" s="31">
+        <v>-5</v>
+      </c>
+      <c r="O40" s="77" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="45"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="76"/>
+      <c r="B41" s="26" t="s">
+        <v>638</v>
+      </c>
+      <c r="C41" s="76" t="s">
+        <v>588</v>
+      </c>
       <c r="D41" s="28"/>
       <c r="E41" s="28"/>
       <c r="F41" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G41" s="29" t="s">
-        <v>526</v>
-      </c>
-      <c r="H41" s="30"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="77"/>
+      <c r="G41" s="76" t="s">
+        <v>517</v>
+      </c>
+      <c r="H41" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I41" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J41" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K41" s="31">
+        <v>32</v>
+      </c>
+      <c r="L41" s="31">
+        <v>2</v>
+      </c>
+      <c r="M41" s="31" t="s">
+        <v>625</v>
+      </c>
+      <c r="N41" s="31">
+        <v>-7</v>
+      </c>
+      <c r="O41" s="77" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="45"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="76"/>
+      <c r="B42" s="26" t="s">
+        <v>644</v>
+      </c>
+      <c r="C42" s="76" t="s">
+        <v>589</v>
+      </c>
       <c r="D42" s="28"/>
       <c r="E42" s="28"/>
       <c r="F42" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G42" s="29" t="s">
-        <v>528</v>
-      </c>
-      <c r="H42" s="30"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="31"/>
-      <c r="N42" s="31"/>
-      <c r="O42" s="77"/>
+      <c r="G42" s="76" t="s">
+        <v>518</v>
+      </c>
+      <c r="H42" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I42" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J42" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K42" s="31">
+        <v>32</v>
+      </c>
+      <c r="L42" s="31">
+        <v>2</v>
+      </c>
+      <c r="M42" s="31" t="s">
+        <v>626</v>
+      </c>
+      <c r="N42" s="31">
+        <v>-16</v>
+      </c>
+      <c r="O42" s="77" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="45"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="76"/>
+      <c r="B43" s="26" t="s">
+        <v>645</v>
+      </c>
+      <c r="C43" s="76" t="s">
+        <v>606</v>
+      </c>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G43" s="29" t="s">
-        <v>527</v>
-      </c>
-      <c r="H43" s="30"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="31"/>
-      <c r="O43" s="77"/>
+      <c r="G43" s="76" t="s">
+        <v>519</v>
+      </c>
+      <c r="H43" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I43" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K43" s="31">
+        <v>32</v>
+      </c>
+      <c r="L43" s="31">
+        <v>1</v>
+      </c>
+      <c r="M43" s="31" t="s">
+        <v>627</v>
+      </c>
+      <c r="N43" s="83">
+        <v>-9</v>
+      </c>
+      <c r="O43" s="77" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="45"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="76"/>
+      <c r="B44" s="26" t="s">
+        <v>645</v>
+      </c>
+      <c r="C44" s="76" t="s">
+        <v>607</v>
+      </c>
       <c r="D44" s="28"/>
       <c r="E44" s="28"/>
       <c r="F44" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G44" s="29" t="s">
-        <v>529</v>
-      </c>
-      <c r="H44" s="30"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="31"/>
-      <c r="M44" s="31"/>
-      <c r="N44" s="31"/>
-      <c r="O44" s="77"/>
+      <c r="G44" s="76" t="s">
+        <v>519</v>
+      </c>
+      <c r="H44" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I44" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J44" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K44" s="31">
+        <v>32</v>
+      </c>
+      <c r="L44" s="31">
+        <v>1</v>
+      </c>
+      <c r="M44" s="31" t="s">
+        <v>621</v>
+      </c>
+      <c r="N44" s="83">
+        <v>-9</v>
+      </c>
+      <c r="O44" s="77" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
+      <c r="A45" s="45"/>
       <c r="B45" s="26" t="s">
-        <v>579</v>
+        <v>651</v>
       </c>
       <c r="C45" s="76" t="s">
-        <v>580</v>
+        <v>608</v>
       </c>
       <c r="D45" s="28"/>
       <c r="E45" s="28"/>
@@ -5044,13 +5611,13 @@
         <v>27</v>
       </c>
       <c r="G45" s="76" t="s">
-        <v>578</v>
-      </c>
-      <c r="H45" s="30" t="s">
-        <v>581</v>
+        <v>519</v>
+      </c>
+      <c r="H45" s="82" t="s">
+        <v>612</v>
       </c>
       <c r="I45" s="28" t="s">
-        <v>35</v>
+        <v>613</v>
       </c>
       <c r="J45" s="31" t="s">
         <v>36</v>
@@ -5059,97 +5626,589 @@
         <v>32</v>
       </c>
       <c r="L45" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M45" s="31" t="s">
-        <v>582</v>
-      </c>
-      <c r="N45" s="31">
-        <v>-1</v>
+        <v>628</v>
+      </c>
+      <c r="N45" s="83">
+        <v>-17.2</v>
       </c>
       <c r="O45" s="77" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="45"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="76"/>
+      <c r="B46" s="26" t="s">
+        <v>648</v>
+      </c>
+      <c r="C46" s="76" t="s">
+        <v>590</v>
+      </c>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
-      <c r="O46" s="77"/>
+      <c r="F46" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="76" t="s">
+        <v>520</v>
+      </c>
+      <c r="H46" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I46" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J46" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K46" s="31">
+        <v>32</v>
+      </c>
+      <c r="L46" s="31">
+        <v>2</v>
+      </c>
+      <c r="M46" s="31" t="s">
+        <v>629</v>
+      </c>
+      <c r="N46" s="31">
+        <v>-28.5</v>
+      </c>
+      <c r="O46" s="77" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="45"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="76"/>
+      <c r="B47" s="26" t="s">
+        <v>649</v>
+      </c>
+      <c r="C47" s="76" t="s">
+        <v>591</v>
+      </c>
       <c r="D47" s="28"/>
       <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
-      <c r="O47" s="77"/>
+      <c r="F47" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="76" t="s">
+        <v>521</v>
+      </c>
+      <c r="H47" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I47" s="28" t="s">
+        <v>614</v>
+      </c>
+      <c r="J47" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K47" s="31">
+        <v>32</v>
+      </c>
+      <c r="L47" s="31">
+        <v>2</v>
+      </c>
+      <c r="M47" s="31" t="s">
+        <v>630</v>
+      </c>
+      <c r="N47" s="31">
+        <v>-4</v>
+      </c>
+      <c r="O47" s="77" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="45"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="76"/>
+      <c r="B48" s="26" t="s">
+        <v>652</v>
+      </c>
+      <c r="C48" s="76" t="s">
+        <v>602</v>
+      </c>
       <c r="D48" s="28"/>
       <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="31"/>
-      <c r="K48" s="31"/>
-      <c r="L48" s="31"/>
-      <c r="M48" s="31"/>
-      <c r="N48" s="31"/>
-      <c r="O48" s="77"/>
-    </row>
-    <row r="49" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="33"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-      <c r="K49" s="34"/>
-      <c r="L49" s="34"/>
-      <c r="M49" s="36"/>
-      <c r="N49" s="34"/>
-      <c r="O49" s="37"/>
-    </row>
-    <row r="50" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="2">
-        <f>COUNTA(D4:D49)</f>
+      <c r="F48" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="H48" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I48" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J48" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K48" s="31">
+        <v>32</v>
+      </c>
+      <c r="L48" s="31">
+        <v>2</v>
+      </c>
+      <c r="M48" s="31" t="s">
+        <v>631</v>
+      </c>
+      <c r="N48" s="31">
+        <v>-0.5</v>
+      </c>
+      <c r="O48" s="77" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="45"/>
+      <c r="B49" s="26" t="s">
+        <v>652</v>
+      </c>
+      <c r="C49" s="76" t="s">
+        <v>592</v>
+      </c>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="H49" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I49" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J49" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K49" s="31">
+        <v>32</v>
+      </c>
+      <c r="L49" s="31">
+        <v>2</v>
+      </c>
+      <c r="M49" s="31" t="s">
+        <v>632</v>
+      </c>
+      <c r="N49" s="31">
+        <v>-20</v>
+      </c>
+      <c r="O49" s="77" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="45"/>
+      <c r="B50" s="26" t="s">
+        <v>653</v>
+      </c>
+      <c r="C50" s="76" t="s">
+        <v>593</v>
+      </c>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="H50" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I50" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J50" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K50" s="31">
+        <v>32</v>
+      </c>
+      <c r="L50" s="31">
+        <v>2</v>
+      </c>
+      <c r="M50" s="31" t="s">
+        <v>633</v>
+      </c>
+      <c r="N50" s="31">
+        <v>-14.5</v>
+      </c>
+      <c r="O50" s="77" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="45"/>
+      <c r="B51" s="26" t="s">
+        <v>657</v>
+      </c>
+      <c r="C51" s="76" t="s">
+        <v>594</v>
+      </c>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G51" s="76" t="s">
+        <v>523</v>
+      </c>
+      <c r="H51" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I51" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J51" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K51" s="31">
+        <v>32</v>
+      </c>
+      <c r="L51" s="31">
+        <v>2</v>
+      </c>
+      <c r="M51" s="31" t="s">
+        <v>634</v>
+      </c>
+      <c r="N51" s="31">
+        <v>-29</v>
+      </c>
+      <c r="O51" s="77" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="45"/>
+      <c r="B52" s="26" t="s">
+        <v>657</v>
+      </c>
+      <c r="C52" s="76" t="s">
+        <v>594</v>
+      </c>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="76" t="s">
+        <v>524</v>
+      </c>
+      <c r="H52" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I52" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J52" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K52" s="31">
+        <v>32</v>
+      </c>
+      <c r="L52" s="31">
+        <v>2</v>
+      </c>
+      <c r="M52" s="31" t="s">
+        <v>634</v>
+      </c>
+      <c r="N52" s="31">
+        <v>-29</v>
+      </c>
+      <c r="O52" s="77" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="45"/>
+      <c r="B53" s="26" t="s">
+        <v>658</v>
+      </c>
+      <c r="C53" s="76" t="s">
+        <v>595</v>
+      </c>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G53" s="76" t="s">
+        <v>525</v>
+      </c>
+      <c r="H53" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I53" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J53" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K53" s="31">
+        <v>32</v>
+      </c>
+      <c r="L53" s="31">
+        <v>2</v>
+      </c>
+      <c r="M53" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="N53" s="31">
+        <v>-10</v>
+      </c>
+      <c r="O53" s="77" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="45"/>
+      <c r="B54" s="26" t="s">
+        <v>658</v>
+      </c>
+      <c r="C54" s="76" t="s">
+        <v>595</v>
+      </c>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G54" s="76" t="s">
+        <v>527</v>
+      </c>
+      <c r="H54" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I54" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J54" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K54" s="31">
+        <v>32</v>
+      </c>
+      <c r="L54" s="31">
+        <v>2</v>
+      </c>
+      <c r="M54" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="N54" s="31">
+        <v>-10</v>
+      </c>
+      <c r="O54" s="77" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="45"/>
+      <c r="B55" s="26" t="s">
+        <v>656</v>
+      </c>
+      <c r="C55" s="76" t="s">
+        <v>596</v>
+      </c>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G55" s="76" t="s">
+        <v>526</v>
+      </c>
+      <c r="H55" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I55" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J55" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K55" s="31">
+        <v>32</v>
+      </c>
+      <c r="L55" s="31">
+        <v>2</v>
+      </c>
+      <c r="M55" s="31" t="s">
+        <v>635</v>
+      </c>
+      <c r="N55" s="31">
+        <v>-13</v>
+      </c>
+      <c r="O55" s="77" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="45"/>
+      <c r="B56" s="26" t="s">
+        <v>650</v>
+      </c>
+      <c r="C56" s="76" t="s">
+        <v>597</v>
+      </c>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56" s="76" t="s">
+        <v>528</v>
+      </c>
+      <c r="H56" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="I56" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="J56" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K56" s="31">
+        <v>32</v>
+      </c>
+      <c r="L56" s="31">
+        <v>2</v>
+      </c>
+      <c r="M56" s="31" t="s">
+        <v>636</v>
+      </c>
+      <c r="N56" s="31">
         <v>0</v>
       </c>
-      <c r="E50" s="2">
-        <f>COUNTA(E4:E49)</f>
+      <c r="O56" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="25"/>
+      <c r="B57" s="26" t="s">
+        <v>578</v>
+      </c>
+      <c r="C57" s="76" t="s">
+        <v>579</v>
+      </c>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G57" s="76" t="s">
+        <v>577</v>
+      </c>
+      <c r="H57" s="30" t="s">
+        <v>580</v>
+      </c>
+      <c r="I57" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="J57" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K57" s="31">
+        <v>32</v>
+      </c>
+      <c r="L57" s="31">
+        <v>1</v>
+      </c>
+      <c r="M57" s="31" t="s">
+        <v>581</v>
+      </c>
+      <c r="N57" s="31">
+        <v>-1</v>
+      </c>
+      <c r="O57" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="45"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="76"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="28"/>
+      <c r="J58" s="31"/>
+      <c r="K58" s="31"/>
+      <c r="L58" s="31"/>
+      <c r="M58" s="31"/>
+      <c r="N58" s="31"/>
+      <c r="O58" s="77"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="45"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="76"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="30"/>
+      <c r="I59" s="28"/>
+      <c r="J59" s="31"/>
+      <c r="K59" s="31"/>
+      <c r="L59" s="31"/>
+      <c r="M59" s="31"/>
+      <c r="N59" s="31"/>
+      <c r="O59" s="77"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="45"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="30"/>
+      <c r="I60" s="28"/>
+      <c r="J60" s="31"/>
+      <c r="K60" s="31"/>
+      <c r="L60" s="31"/>
+      <c r="M60" s="31"/>
+      <c r="N60" s="31"/>
+      <c r="O60" s="77"/>
+    </row>
+    <row r="61" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="33"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="34"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="34"/>
+      <c r="J61" s="34"/>
+      <c r="K61" s="34"/>
+      <c r="L61" s="34"/>
+      <c r="M61" s="36"/>
+      <c r="N61" s="34"/>
+      <c r="O61" s="37"/>
+    </row>
+    <row r="62" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="2">
+        <f>COUNTA(D4:D61)</f>
         <v>0</v>
       </c>
-      <c r="F50" s="2">
-        <f>COUNTA(F4:F49)</f>
-        <v>42</v>
+      <c r="E62" s="2">
+        <f>COUNTA(E4:E61)</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="2">
+        <f>COUNTA(F4:F61)</f>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -5211,16 +6270,96 @@
     <hyperlink ref="C27" r:id="rId55"/>
     <hyperlink ref="C28" r:id="rId56"/>
     <hyperlink ref="O27" r:id="rId57" location="'Niveles'!B9"/>
-    <hyperlink ref="G35" r:id="rId58"/>
-    <hyperlink ref="G29" r:id="rId59"/>
-    <hyperlink ref="G30" r:id="rId60"/>
-    <hyperlink ref="C45" r:id="rId61"/>
-    <hyperlink ref="G45" r:id="rId62"/>
-    <hyperlink ref="O45" r:id="rId63" location="'Niveles'!B14"/>
+    <hyperlink ref="G46" r:id="rId58"/>
+    <hyperlink ref="G34" r:id="rId59"/>
+    <hyperlink ref="G36" r:id="rId60"/>
+    <hyperlink ref="C57" r:id="rId61"/>
+    <hyperlink ref="G57" r:id="rId62"/>
+    <hyperlink ref="O57" r:id="rId63" location="'Niveles'!B14"/>
     <hyperlink ref="O28" r:id="rId64" location="'Niveles'!B15"/>
+    <hyperlink ref="G40" r:id="rId65"/>
+    <hyperlink ref="C36" r:id="rId66"/>
+    <hyperlink ref="C40" r:id="rId67"/>
+    <hyperlink ref="G41" r:id="rId68"/>
+    <hyperlink ref="C41" r:id="rId69"/>
+    <hyperlink ref="G42" r:id="rId70"/>
+    <hyperlink ref="C42" r:id="rId71"/>
+    <hyperlink ref="G45" r:id="rId72"/>
+    <hyperlink ref="C46" r:id="rId73"/>
+    <hyperlink ref="C47" r:id="rId74"/>
+    <hyperlink ref="G50" r:id="rId75"/>
+    <hyperlink ref="C50" r:id="rId76"/>
+    <hyperlink ref="G49" r:id="rId77"/>
+    <hyperlink ref="C49" r:id="rId78"/>
+    <hyperlink ref="G51" r:id="rId79"/>
+    <hyperlink ref="G52" r:id="rId80"/>
+    <hyperlink ref="G53" r:id="rId81"/>
+    <hyperlink ref="G54" r:id="rId82"/>
+    <hyperlink ref="C52" r:id="rId83"/>
+    <hyperlink ref="G55" r:id="rId84"/>
+    <hyperlink ref="C54" r:id="rId85"/>
+    <hyperlink ref="C51" r:id="rId86"/>
+    <hyperlink ref="C55" r:id="rId87"/>
+    <hyperlink ref="G56" r:id="rId88"/>
+    <hyperlink ref="C56" r:id="rId89"/>
+    <hyperlink ref="G35" r:id="rId90"/>
+    <hyperlink ref="C35" r:id="rId91"/>
+    <hyperlink ref="G37" r:id="rId92"/>
+    <hyperlink ref="C37" r:id="rId93"/>
+    <hyperlink ref="G38" r:id="rId94"/>
+    <hyperlink ref="C38" r:id="rId95"/>
+    <hyperlink ref="G39" r:id="rId96"/>
+    <hyperlink ref="C39" r:id="rId97"/>
+    <hyperlink ref="G48" r:id="rId98"/>
+    <hyperlink ref="C48" r:id="rId99"/>
+    <hyperlink ref="C34" r:id="rId100"/>
+    <hyperlink ref="G32" r:id="rId101"/>
+    <hyperlink ref="C32" r:id="rId102"/>
+    <hyperlink ref="G33" r:id="rId103"/>
+    <hyperlink ref="C33" r:id="rId104"/>
+    <hyperlink ref="C53" r:id="rId105"/>
+    <hyperlink ref="C45" r:id="rId106"/>
+    <hyperlink ref="G43" r:id="rId107"/>
+    <hyperlink ref="C43" r:id="rId108"/>
+    <hyperlink ref="G44" r:id="rId109"/>
+    <hyperlink ref="C44" r:id="rId110"/>
+    <hyperlink ref="C31" r:id="rId111"/>
+    <hyperlink ref="C30" r:id="rId112"/>
+    <hyperlink ref="C29" r:id="rId113"/>
+    <hyperlink ref="H29" r:id="rId114"/>
+    <hyperlink ref="H30:H56" r:id="rId115" display="Revisable en el .aup en: Docs/TDS/Credits/"/>
+    <hyperlink ref="G47" r:id="rId116"/>
+    <hyperlink ref="O37" r:id="rId117" location="'Creditos'!B7"/>
+    <hyperlink ref="O36" r:id="rId118" location="'Creditos'!B7"/>
+    <hyperlink ref="O41" r:id="rId119" location="'Creditos'!B8"/>
+    <hyperlink ref="O38" r:id="rId120" location="'Creditos'!B12"/>
+    <hyperlink ref="O35" r:id="rId121" location="'Creditos'!B13"/>
+    <hyperlink ref="O39" r:id="rId122" location="'Creditos'!B14"/>
+    <hyperlink ref="O40" r:id="rId123" location="'Creditos'!B15"/>
+    <hyperlink ref="O42" r:id="rId124" location="'Creditos'!B18"/>
+    <hyperlink ref="O44" r:id="rId125" location="'Creditos'!B22"/>
+    <hyperlink ref="O31" r:id="rId126" location="'Creditos'!B17"/>
+    <hyperlink ref="O30" r:id="rId127" location="'Creditos'!B19"/>
+    <hyperlink ref="O46" r:id="rId128" location="'Creditos'!B21"/>
+    <hyperlink ref="O47" r:id="rId129" location="'Creditos'!B24"/>
+    <hyperlink ref="O56" r:id="rId130" location="'Creditos'!B25"/>
+    <hyperlink ref="O45" r:id="rId131" location="'Creditos'!B27"/>
+    <hyperlink ref="O49" r:id="rId132" location="'Creditos'!B28"/>
+    <hyperlink ref="O50" r:id="rId133" location="'Creditos'!B30"/>
+    <hyperlink ref="O29" r:id="rId134" location="'Creditos'!B31"/>
+    <hyperlink ref="O34" r:id="rId135" location="'Creditos'!B32"/>
+    <hyperlink ref="O55" r:id="rId136" location="'Creditos'!B34"/>
+    <hyperlink ref="O53" r:id="rId137" location="'Creditos'!B38"/>
+    <hyperlink ref="O54" r:id="rId138" location="'Creditos'!B38"/>
+    <hyperlink ref="O32" r:id="rId139" location="'Creditos'!B11"/>
+    <hyperlink ref="O51" r:id="rId140" location="'Creditos'!B35"/>
+    <hyperlink ref="O33" r:id="rId141" location="'Creditos'!B11"/>
+    <hyperlink ref="O43" r:id="rId142" location="'Creditos'!B22"/>
+    <hyperlink ref="O48" r:id="rId143" location="'Creditos'!B28"/>
+    <hyperlink ref="O52" r:id="rId144" location="'Creditos'!B35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId145"/>
 </worksheet>
 </file>
 
@@ -5328,10 +6467,10 @@
     </row>
     <row r="4" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="38" t="s">
+        <v>543</v>
+      </c>
+      <c r="C4" s="79" t="s">
         <v>544</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>545</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>25</v>
@@ -5339,10 +6478,10 @@
       <c r="E4" s="40"/>
       <c r="F4" s="40"/>
       <c r="G4" s="80" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I4" s="28" t="s">
         <v>35</v>
@@ -5357,7 +6496,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="42" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="N4" s="42">
         <v>-2</v>
@@ -5368,10 +6507,10 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="52" t="s">
+        <v>547</v>
+      </c>
+      <c r="C5" s="76" t="s">
         <v>548</v>
-      </c>
-      <c r="C5" s="76" t="s">
-        <v>549</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>25</v>
@@ -5379,10 +6518,10 @@
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
       <c r="G5" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I5" s="28" t="s">
         <v>35</v>
@@ -5397,7 +6536,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="31" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="N5" s="31">
         <v>-2</v>
@@ -5408,10 +6547,10 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="52" t="s">
+        <v>551</v>
+      </c>
+      <c r="C6" s="76" t="s">
         <v>552</v>
-      </c>
-      <c r="C6" s="76" t="s">
-        <v>553</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>25</v>
@@ -5419,10 +6558,10 @@
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
       <c r="G6" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I6" s="28" t="s">
         <v>35</v>
@@ -5437,7 +6576,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="31" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="N6" s="31">
         <v>-2</v>
@@ -5448,10 +6587,10 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="52" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C7" s="76" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>25</v>
@@ -5459,10 +6598,10 @@
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
       <c r="G7" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I7" s="28" t="s">
         <v>35</v>
@@ -5477,7 +6616,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="31" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="N7" s="31">
         <v>-2</v>
@@ -5488,10 +6627,10 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="52" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C8" s="76" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>25</v>
@@ -5499,10 +6638,10 @@
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
       <c r="G8" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I8" s="28" t="s">
         <v>35</v>
@@ -5517,7 +6656,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="31" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N8" s="31">
         <v>-2</v>
@@ -5528,10 +6667,10 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="52" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C9" s="76" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>25</v>
@@ -5539,10 +6678,10 @@
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
       <c r="G9" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I9" s="28" t="s">
         <v>35</v>
@@ -5557,7 +6696,7 @@
         <v>1</v>
       </c>
       <c r="M9" s="31" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="N9" s="31">
         <v>-2</v>
@@ -5568,10 +6707,10 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="52" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C10" s="76" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>25</v>
@@ -5579,10 +6718,10 @@
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I10" s="28" t="s">
         <v>35</v>
@@ -5597,21 +6736,21 @@
         <v>1</v>
       </c>
       <c r="M10" s="31" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="N10" s="31">
         <v>-17</v>
       </c>
       <c r="O10" s="77" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="52" t="s">
+        <v>564</v>
+      </c>
+      <c r="C11" s="76" t="s">
         <v>565</v>
-      </c>
-      <c r="C11" s="76" t="s">
-        <v>566</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>25</v>
@@ -5619,10 +6758,10 @@
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
       <c r="G11" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I11" s="28" t="s">
         <v>35</v>
@@ -5637,7 +6776,7 @@
         <v>1</v>
       </c>
       <c r="M11" s="31" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="N11" s="31">
         <v>-13</v>
@@ -5648,10 +6787,10 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="52" t="s">
+        <v>568</v>
+      </c>
+      <c r="C12" s="76" t="s">
         <v>569</v>
-      </c>
-      <c r="C12" s="76" t="s">
-        <v>570</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>25</v>
@@ -5659,10 +6798,10 @@
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
       <c r="G12" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I12" s="28" t="s">
         <v>35</v>
@@ -5677,21 +6816,21 @@
         <v>1</v>
       </c>
       <c r="M12" s="31" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="N12" s="31">
         <v>-3</v>
       </c>
       <c r="O12" s="77" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C13" s="76" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>25</v>
@@ -5699,10 +6838,10 @@
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I13" s="28" t="s">
         <v>35</v>
@@ -5717,7 +6856,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="31" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="N13" s="31">
         <v>-14</v>
@@ -5728,10 +6867,10 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="C14" s="76" t="s">
         <v>575</v>
-      </c>
-      <c r="C14" s="76" t="s">
-        <v>576</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>25</v>
@@ -5739,10 +6878,10 @@
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
       <c r="G14" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I14" s="28" t="s">
         <v>35</v>
@@ -5757,7 +6896,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="31" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="N14" s="31">
         <v>-16</v>
@@ -6053,10 +7192,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C7" s="76" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D7" s="28"/>
       <c r="E7" s="28" t="s">
@@ -6088,15 +7227,15 @@
         <v>-10.5</v>
       </c>
       <c r="O7" s="77" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C8" s="76" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28" t="s">
@@ -6107,7 +7246,7 @@
         <v>157</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I8" s="28" t="s">
         <v>35</v>
@@ -6122,7 +7261,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="31" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="N8" s="31">
         <v>-8</v>
@@ -6133,10 +7272,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
+        <v>536</v>
+      </c>
+      <c r="C9" s="76" t="s">
         <v>537</v>
-      </c>
-      <c r="C9" s="76" t="s">
-        <v>538</v>
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="28" t="s">
@@ -6162,21 +7301,21 @@
         <v>1</v>
       </c>
       <c r="M9" s="31" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="N9" s="31">
         <v>-3</v>
       </c>
       <c r="O9" s="77" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
+        <v>540</v>
+      </c>
+      <c r="C10" s="76" t="s">
         <v>541</v>
-      </c>
-      <c r="C10" s="76" t="s">
-        <v>542</v>
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="28" t="s">
@@ -6202,7 +7341,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="31" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="N10" s="31">
         <v>0</v>
@@ -6213,10 +7352,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
+        <v>582</v>
+      </c>
+      <c r="C11" s="76" t="s">
         <v>583</v>
-      </c>
-      <c r="C11" s="76" t="s">
-        <v>584</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28" t="s">
@@ -6227,7 +7366,7 @@
         <v>157</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I11" s="28" t="s">
         <v>35</v>
@@ -6242,13 +7381,13 @@
         <v>1</v>
       </c>
       <c r="M11" s="31" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="N11" s="31">
         <v>-18.5</v>
       </c>
       <c r="O11" s="77" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>